<commit_message>
more named cells, fixed A-sheet results, added Pas-de-deux
</commit_message>
<xml_diff>
--- a/mallar/Protokoll 2017 individuell klass_justerat 2017-05-30.xlsx
+++ b/mallar/Protokoll 2017 individuell klass_justerat 2017-05-30.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="PdI6n2wWe1BCLpZSUVKb6Viv2S5eDDxdev/RLVBc6uGkqKIeSnzxpXt+L8Ip+7bcU/gK26fAQjqxcl2KM0Nr6Q==" workbookSaltValue="84UlA07g1xLdi6rLqV4A4w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="10320" windowHeight="7650" tabRatio="941" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="10320" windowHeight="7650" tabRatio="941"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="37" r:id="rId1"/>
@@ -61,7 +61,7 @@
     <definedName name="moment" localSheetId="4">'Individuell senior grund 3'!$L$5</definedName>
     <definedName name="moment" localSheetId="8">'Individuell tekniska övningar'!$L$5</definedName>
     <definedName name="moment" localSheetId="9">'Individuellt tekniskt artistisk'!$L$6</definedName>
-    <definedName name="result" localSheetId="1">'Häst, individuell'!$K$25:$L$25</definedName>
+    <definedName name="result" localSheetId="1">'Häst, individuell'!$K$25</definedName>
     <definedName name="result" localSheetId="5">'Ind kür tekn 1'!$L$33</definedName>
     <definedName name="result" localSheetId="6">'Ind kür tekn 2 3'!$L$33</definedName>
     <definedName name="result" localSheetId="3">'Individuell junior grund 2'!$L$27</definedName>
@@ -2838,6 +2838,96 @@
     <xf numFmtId="167" fontId="1" fillId="4" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="49" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="52" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="47" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="46" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="173" fontId="2" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2856,12 +2946,6 @@
     <xf numFmtId="167" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="173" fontId="2" fillId="4" borderId="47" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2877,90 +2961,6 @@
     <xf numFmtId="167" fontId="1" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="46" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="49" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="52" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="47" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3057,50 +3057,50 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -3456,7 +3456,7 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:Q84"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A26" workbookViewId="0">
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="A26" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -5409,17 +5409,17 @@
   <sheetData>
     <row r="1" spans="1:12" s="151" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:12" s="7" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="452" t="s">
+      <c r="A2" s="450" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="452"/>
-      <c r="C2" s="452"/>
-      <c r="D2" s="452"/>
-      <c r="E2" s="452"/>
-      <c r="F2" s="452"/>
-      <c r="G2" s="452"/>
-      <c r="H2" s="452"/>
-      <c r="I2" s="452"/>
+      <c r="B2" s="450"/>
+      <c r="C2" s="450"/>
+      <c r="D2" s="450"/>
+      <c r="E2" s="450"/>
+      <c r="F2" s="450"/>
+      <c r="G2" s="450"/>
+      <c r="H2" s="450"/>
+      <c r="I2" s="450"/>
       <c r="J2" s="186"/>
       <c r="K2" s="186"/>
       <c r="L2" s="186"/>
@@ -5464,10 +5464,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="388"/>
-      <c r="D5" s="388"/>
-      <c r="E5" s="388"/>
-      <c r="F5" s="388"/>
+      <c r="C5" s="399"/>
+      <c r="D5" s="399"/>
+      <c r="E5" s="399"/>
+      <c r="F5" s="399"/>
       <c r="G5" s="185"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
@@ -5482,10 +5482,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="388"/>
-      <c r="D6" s="388"/>
-      <c r="E6" s="388"/>
-      <c r="F6" s="388"/>
+      <c r="C6" s="399"/>
+      <c r="D6" s="399"/>
+      <c r="E6" s="399"/>
+      <c r="F6" s="399"/>
       <c r="G6" s="184"/>
       <c r="H6" s="141"/>
       <c r="I6" s="17" t="s">
@@ -5534,10 +5534,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="388"/>
-      <c r="D9" s="388"/>
-      <c r="E9" s="388"/>
-      <c r="F9" s="388"/>
+      <c r="C9" s="399"/>
+      <c r="D9" s="399"/>
+      <c r="E9" s="399"/>
+      <c r="F9" s="399"/>
       <c r="G9" s="206"/>
       <c r="H9" s="183"/>
       <c r="I9" s="183"/>
@@ -5550,15 +5550,15 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="388"/>
-      <c r="D10" s="388"/>
-      <c r="E10" s="388"/>
-      <c r="F10" s="388"/>
+      <c r="C10" s="399"/>
+      <c r="D10" s="399"/>
+      <c r="E10" s="399"/>
+      <c r="F10" s="399"/>
       <c r="G10" s="206"/>
       <c r="H10" s="183"/>
       <c r="I10" s="183"/>
-      <c r="J10" s="448"/>
-      <c r="K10" s="448"/>
+      <c r="J10" s="446"/>
+      <c r="K10" s="446"/>
       <c r="L10" s="207"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -5585,10 +5585,10 @@
       <c r="C13" s="343" t="s">
         <v>181</v>
       </c>
-      <c r="D13" s="453" t="s">
+      <c r="D13" s="451" t="s">
         <v>182</v>
       </c>
-      <c r="E13" s="454"/>
+      <c r="E13" s="452"/>
       <c r="F13" s="343" t="s">
         <v>183</v>
       </c>
@@ -5601,17 +5601,17 @@
       <c r="I13" s="345" t="s">
         <v>144</v>
       </c>
-      <c r="J13" s="457" t="s">
+      <c r="J13" s="455" t="s">
         <v>190</v>
       </c>
-      <c r="K13" s="458"/>
+      <c r="K13" s="456"/>
       <c r="L13" s="205"/>
     </row>
     <row r="14" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="368"/>
       <c r="C14" s="369"/>
-      <c r="D14" s="455"/>
-      <c r="E14" s="456"/>
+      <c r="D14" s="453"/>
+      <c r="E14" s="454"/>
       <c r="F14" s="369"/>
       <c r="G14" s="369"/>
       <c r="H14" s="370"/>
@@ -5619,11 +5619,11 @@
         <f>SUM(B14:H14)</f>
         <v>0</v>
       </c>
-      <c r="J14" s="459">
+      <c r="J14" s="457">
         <f>I14/6</f>
         <v>0</v>
       </c>
-      <c r="K14" s="460"/>
+      <c r="K14" s="458"/>
       <c r="L14" s="205"/>
     </row>
     <row r="15" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5652,16 +5652,16 @@
       <c r="A17" s="334" t="s">
         <v>189</v>
       </c>
-      <c r="B17" s="449" t="s">
+      <c r="B17" s="447" t="s">
         <v>186</v>
       </c>
-      <c r="C17" s="450"/>
-      <c r="D17" s="450"/>
-      <c r="E17" s="450"/>
-      <c r="F17" s="450"/>
-      <c r="G17" s="450"/>
-      <c r="H17" s="450"/>
-      <c r="I17" s="451"/>
+      <c r="C17" s="448"/>
+      <c r="D17" s="448"/>
+      <c r="E17" s="448"/>
+      <c r="F17" s="448"/>
+      <c r="G17" s="448"/>
+      <c r="H17" s="448"/>
+      <c r="I17" s="449"/>
       <c r="J17" s="203" t="s">
         <v>187</v>
       </c>
@@ -5675,7 +5675,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="446" t="s">
+      <c r="A18" s="459" t="s">
         <v>91</v>
       </c>
       <c r="B18" s="425" t="s">
@@ -5698,7 +5698,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="447"/>
+      <c r="A19" s="460"/>
       <c r="B19" s="427" t="s">
         <v>167</v>
       </c>
@@ -5838,6 +5838,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="A2:I2"/>
@@ -5847,12 +5853,6 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="J14:K14"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5868,7 +5868,7 @@
   <sheetPr codeName="Blad2"/>
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K19" sqref="K19:K23"/>
     </sheetView>
   </sheetViews>
@@ -5937,10 +5937,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="14"/>
-      <c r="C4" s="388"/>
-      <c r="D4" s="388"/>
-      <c r="E4" s="388"/>
-      <c r="F4" s="388"/>
+      <c r="C4" s="399"/>
+      <c r="D4" s="399"/>
+      <c r="E4" s="399"/>
+      <c r="F4" s="399"/>
       <c r="H4" s="16"/>
       <c r="I4" s="17" t="s">
         <v>14</v>
@@ -5954,10 +5954,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="388"/>
-      <c r="D5" s="388"/>
-      <c r="E5" s="388"/>
-      <c r="F5" s="388"/>
+      <c r="C5" s="399"/>
+      <c r="D5" s="399"/>
+      <c r="E5" s="399"/>
+      <c r="F5" s="399"/>
       <c r="K5" s="56"/>
     </row>
     <row r="6" spans="1:12" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5982,10 +5982,10 @@
         <v>0</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="388"/>
-      <c r="D7" s="388"/>
-      <c r="E7" s="388"/>
-      <c r="F7" s="388"/>
+      <c r="C7" s="399"/>
+      <c r="D7" s="399"/>
+      <c r="E7" s="399"/>
+      <c r="F7" s="399"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -5997,10 +5997,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="14"/>
-      <c r="C8" s="388"/>
-      <c r="D8" s="388"/>
-      <c r="E8" s="388"/>
-      <c r="F8" s="388"/>
+      <c r="C8" s="399"/>
+      <c r="D8" s="399"/>
+      <c r="E8" s="399"/>
+      <c r="F8" s="399"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -6012,10 +6012,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="388"/>
-      <c r="D9" s="388"/>
-      <c r="E9" s="388"/>
-      <c r="F9" s="388"/>
+      <c r="C9" s="399"/>
+      <c r="D9" s="399"/>
+      <c r="E9" s="399"/>
+      <c r="F9" s="399"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -6049,215 +6049,215 @@
       <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H12" s="389" t="s">
+      <c r="H12" s="400" t="s">
         <v>42</v>
       </c>
-      <c r="I12" s="390"/>
-      <c r="J12" s="391" t="s">
+      <c r="I12" s="401"/>
+      <c r="J12" s="402" t="s">
         <v>43</v>
       </c>
-      <c r="K12" s="391"/>
-      <c r="L12" s="391"/>
+      <c r="K12" s="402"/>
+      <c r="L12" s="402"/>
     </row>
     <row r="13" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="392" t="s">
+      <c r="A13" s="376" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="395" t="s">
+      <c r="B13" s="382" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="395" t="s">
+      <c r="C13" s="382" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="395"/>
-      <c r="E13" s="395"/>
-      <c r="F13" s="397" t="s">
+      <c r="D13" s="382"/>
+      <c r="E13" s="382"/>
+      <c r="F13" s="391" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="398"/>
+      <c r="G13" s="392"/>
       <c r="H13" s="21"/>
       <c r="I13" s="22"/>
-      <c r="J13" s="379" t="s">
+      <c r="J13" s="393" t="s">
         <v>1</v>
       </c>
-      <c r="K13" s="381"/>
-      <c r="L13" s="375">
+      <c r="K13" s="409"/>
+      <c r="L13" s="405">
         <f>ROUND(K13*0.3,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="393"/>
-      <c r="B14" s="396"/>
-      <c r="C14" s="396" t="s">
+      <c r="A14" s="377"/>
+      <c r="B14" s="387"/>
+      <c r="C14" s="387" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="396"/>
-      <c r="E14" s="396"/>
-      <c r="F14" s="399" t="s">
+      <c r="D14" s="387"/>
+      <c r="E14" s="387"/>
+      <c r="F14" s="388" t="s">
         <v>159</v>
       </c>
-      <c r="G14" s="400"/>
+      <c r="G14" s="389"/>
       <c r="H14" s="24"/>
       <c r="I14" s="25"/>
-      <c r="J14" s="380"/>
-      <c r="K14" s="382"/>
-      <c r="L14" s="376"/>
+      <c r="J14" s="394"/>
+      <c r="K14" s="410"/>
+      <c r="L14" s="406"/>
     </row>
     <row r="15" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="393"/>
-      <c r="B15" s="396"/>
-      <c r="C15" s="396" t="s">
+      <c r="A15" s="377"/>
+      <c r="B15" s="387"/>
+      <c r="C15" s="387" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="396"/>
-      <c r="E15" s="396"/>
-      <c r="F15" s="399" t="s">
+      <c r="D15" s="387"/>
+      <c r="E15" s="387"/>
+      <c r="F15" s="388" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="400"/>
+      <c r="G15" s="389"/>
       <c r="H15" s="27"/>
       <c r="I15" s="28"/>
-      <c r="J15" s="380"/>
-      <c r="K15" s="383"/>
-      <c r="L15" s="376"/>
+      <c r="J15" s="394"/>
+      <c r="K15" s="411"/>
+      <c r="L15" s="406"/>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="393"/>
-      <c r="B16" s="401" t="s">
+      <c r="A16" s="377"/>
+      <c r="B16" s="395" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="396" t="s">
+      <c r="C16" s="387" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="396"/>
-      <c r="E16" s="396"/>
-      <c r="F16" s="399" t="s">
+      <c r="D16" s="387"/>
+      <c r="E16" s="387"/>
+      <c r="F16" s="388" t="s">
         <v>160</v>
       </c>
-      <c r="G16" s="400"/>
+      <c r="G16" s="389"/>
       <c r="H16" s="29"/>
       <c r="I16" s="30"/>
-      <c r="J16" s="380" t="s">
+      <c r="J16" s="394" t="s">
         <v>2</v>
       </c>
-      <c r="K16" s="374"/>
-      <c r="L16" s="376">
+      <c r="K16" s="404"/>
+      <c r="L16" s="406">
         <f>ROUND(K16*0.25,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="393"/>
-      <c r="B17" s="402"/>
-      <c r="C17" s="396" t="s">
+      <c r="A17" s="377"/>
+      <c r="B17" s="396"/>
+      <c r="C17" s="387" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="396"/>
-      <c r="E17" s="396"/>
-      <c r="F17" s="399" t="s">
+      <c r="D17" s="387"/>
+      <c r="E17" s="387"/>
+      <c r="F17" s="388" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="400"/>
+      <c r="G17" s="389"/>
       <c r="H17" s="24"/>
       <c r="I17" s="25"/>
-      <c r="J17" s="380"/>
-      <c r="K17" s="374"/>
-      <c r="L17" s="376"/>
+      <c r="J17" s="394"/>
+      <c r="K17" s="404"/>
+      <c r="L17" s="406"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="394"/>
-      <c r="B18" s="403"/>
-      <c r="C18" s="405" t="s">
+      <c r="A18" s="378"/>
+      <c r="B18" s="397"/>
+      <c r="C18" s="390" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="405"/>
-      <c r="E18" s="405"/>
-      <c r="F18" s="386" t="s">
+      <c r="D18" s="390"/>
+      <c r="E18" s="390"/>
+      <c r="F18" s="385" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="387"/>
+      <c r="G18" s="386"/>
       <c r="H18" s="31"/>
       <c r="I18" s="32"/>
-      <c r="J18" s="404"/>
-      <c r="K18" s="384"/>
-      <c r="L18" s="385"/>
+      <c r="J18" s="398"/>
+      <c r="K18" s="412"/>
+      <c r="L18" s="413"/>
     </row>
     <row r="19" spans="1:12" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="392" t="s">
+      <c r="A19" s="376" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="409" t="s">
+      <c r="B19" s="379" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="395" t="s">
+      <c r="C19" s="382" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="395"/>
-      <c r="E19" s="395"/>
-      <c r="F19" s="412" t="s">
+      <c r="D19" s="382"/>
+      <c r="E19" s="382"/>
+      <c r="F19" s="383" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="413"/>
+      <c r="G19" s="384"/>
       <c r="H19" s="33"/>
       <c r="I19" s="34"/>
-      <c r="J19" s="379" t="s">
+      <c r="J19" s="393" t="s">
         <v>104</v>
       </c>
-      <c r="K19" s="373"/>
-      <c r="L19" s="375">
+      <c r="K19" s="403"/>
+      <c r="L19" s="405">
         <f>ROUND(K19*0.25,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="393"/>
-      <c r="B20" s="410"/>
-      <c r="C20" s="396" t="s">
+      <c r="A20" s="377"/>
+      <c r="B20" s="380"/>
+      <c r="C20" s="387" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="396"/>
-      <c r="E20" s="396"/>
-      <c r="F20" s="399" t="s">
+      <c r="D20" s="387"/>
+      <c r="E20" s="387"/>
+      <c r="F20" s="388" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="400"/>
+      <c r="G20" s="389"/>
       <c r="H20" s="24"/>
       <c r="I20" s="25"/>
-      <c r="J20" s="380"/>
-      <c r="K20" s="374"/>
-      <c r="L20" s="376"/>
+      <c r="J20" s="394"/>
+      <c r="K20" s="404"/>
+      <c r="L20" s="406"/>
     </row>
     <row r="21" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="393"/>
-      <c r="B21" s="411"/>
-      <c r="C21" s="396" t="s">
+      <c r="A21" s="377"/>
+      <c r="B21" s="381"/>
+      <c r="C21" s="387" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="396"/>
-      <c r="E21" s="396"/>
-      <c r="F21" s="399" t="s">
+      <c r="D21" s="387"/>
+      <c r="E21" s="387"/>
+      <c r="F21" s="388" t="s">
         <v>34</v>
       </c>
-      <c r="G21" s="400"/>
+      <c r="G21" s="389"/>
       <c r="H21" s="27"/>
       <c r="I21" s="28"/>
-      <c r="J21" s="380"/>
-      <c r="K21" s="374"/>
-      <c r="L21" s="376"/>
+      <c r="J21" s="394"/>
+      <c r="K21" s="404"/>
+      <c r="L21" s="406"/>
     </row>
     <row r="22" spans="1:12" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="394"/>
+      <c r="A22" s="378"/>
       <c r="B22" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="405"/>
-      <c r="D22" s="405"/>
-      <c r="E22" s="405"/>
-      <c r="F22" s="386" t="s">
+      <c r="C22" s="390"/>
+      <c r="D22" s="390"/>
+      <c r="E22" s="390"/>
+      <c r="F22" s="385" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="387"/>
+      <c r="G22" s="386"/>
       <c r="H22" s="36"/>
       <c r="I22" s="37"/>
       <c r="J22" s="38" t="s">
@@ -6276,15 +6276,15 @@
       <c r="B23" s="144" t="s">
         <v>102</v>
       </c>
-      <c r="C23" s="406" t="s">
+      <c r="C23" s="373" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="406"/>
-      <c r="E23" s="406"/>
-      <c r="F23" s="407" t="s">
+      <c r="D23" s="373"/>
+      <c r="E23" s="373"/>
+      <c r="F23" s="374" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="408"/>
+      <c r="G23" s="375"/>
       <c r="H23" s="40"/>
       <c r="I23" s="41"/>
       <c r="J23" s="42" t="s">
@@ -6323,11 +6323,11 @@
         <v>6</v>
       </c>
       <c r="J25" s="46"/>
-      <c r="K25" s="377">
+      <c r="K25" s="407">
         <f>SUM(L13:L23)</f>
         <v>0</v>
       </c>
-      <c r="L25" s="378"/>
+      <c r="L25" s="408"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="K26" s="331"/>
@@ -6354,18 +6354,22 @@
     <row r="30" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="K19:K21"/>
+    <mergeCell ref="L19:L21"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="J19:J21"/>
+    <mergeCell ref="K13:K15"/>
+    <mergeCell ref="L13:L15"/>
+    <mergeCell ref="K16:K18"/>
+    <mergeCell ref="L16:L18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
     <mergeCell ref="A13:A18"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="C13:E13"/>
@@ -6382,22 +6386,18 @@
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="K19:K21"/>
-    <mergeCell ref="L19:L21"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="J19:J21"/>
-    <mergeCell ref="K13:K15"/>
-    <mergeCell ref="L13:L15"/>
-    <mergeCell ref="K16:K18"/>
-    <mergeCell ref="L16:L18"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="C22:E22"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6945,10 +6945,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="388"/>
-      <c r="D5" s="388"/>
-      <c r="E5" s="388"/>
-      <c r="F5" s="388"/>
+      <c r="C5" s="399"/>
+      <c r="D5" s="399"/>
+      <c r="E5" s="399"/>
+      <c r="F5" s="399"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
         <v>14</v>
@@ -6962,10 +6962,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="388"/>
-      <c r="D6" s="388"/>
-      <c r="E6" s="388"/>
-      <c r="F6" s="388"/>
+      <c r="C6" s="399"/>
+      <c r="D6" s="399"/>
+      <c r="E6" s="399"/>
+      <c r="F6" s="399"/>
       <c r="K6" s="56"/>
     </row>
     <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7005,10 +7005,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="388"/>
-      <c r="D9" s="388"/>
-      <c r="E9" s="388"/>
-      <c r="F9" s="388"/>
+      <c r="C9" s="399"/>
+      <c r="D9" s="399"/>
+      <c r="E9" s="399"/>
+      <c r="F9" s="399"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -7020,10 +7020,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="388"/>
-      <c r="D10" s="388"/>
-      <c r="E10" s="388"/>
-      <c r="F10" s="388"/>
+      <c r="C10" s="399"/>
+      <c r="D10" s="399"/>
+      <c r="E10" s="399"/>
+      <c r="F10" s="399"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -7413,10 +7413,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="388"/>
-      <c r="D5" s="388"/>
-      <c r="E5" s="388"/>
-      <c r="F5" s="388"/>
+      <c r="C5" s="399"/>
+      <c r="D5" s="399"/>
+      <c r="E5" s="399"/>
+      <c r="F5" s="399"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
         <v>14</v>
@@ -7430,10 +7430,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="388"/>
-      <c r="D6" s="388"/>
-      <c r="E6" s="388"/>
-      <c r="F6" s="388"/>
+      <c r="C6" s="399"/>
+      <c r="D6" s="399"/>
+      <c r="E6" s="399"/>
+      <c r="F6" s="399"/>
       <c r="K6" s="56"/>
     </row>
     <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7473,10 +7473,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="388"/>
-      <c r="D9" s="388"/>
-      <c r="E9" s="388"/>
-      <c r="F9" s="388"/>
+      <c r="C9" s="399"/>
+      <c r="D9" s="399"/>
+      <c r="E9" s="399"/>
+      <c r="F9" s="399"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -7488,10 +7488,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="388"/>
-      <c r="D10" s="388"/>
-      <c r="E10" s="388"/>
-      <c r="F10" s="388"/>
+      <c r="C10" s="399"/>
+      <c r="D10" s="399"/>
+      <c r="E10" s="399"/>
+      <c r="F10" s="399"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -8309,7 +8309,7 @@
   <sheetPr codeName="Blad7"/>
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
@@ -9007,10 +9007,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="388"/>
-      <c r="D5" s="388"/>
-      <c r="E5" s="388"/>
-      <c r="F5" s="388"/>
+      <c r="C5" s="399"/>
+      <c r="D5" s="399"/>
+      <c r="E5" s="399"/>
+      <c r="F5" s="399"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
         <v>14</v>
@@ -9024,10 +9024,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="388"/>
-      <c r="D6" s="388"/>
-      <c r="E6" s="388"/>
-      <c r="F6" s="388"/>
+      <c r="C6" s="399"/>
+      <c r="D6" s="399"/>
+      <c r="E6" s="399"/>
+      <c r="F6" s="399"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -9071,10 +9071,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="388"/>
-      <c r="D9" s="388"/>
-      <c r="E9" s="388"/>
-      <c r="F9" s="388"/>
+      <c r="C9" s="399"/>
+      <c r="D9" s="399"/>
+      <c r="E9" s="399"/>
+      <c r="F9" s="399"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
@@ -9086,10 +9086,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="388"/>
-      <c r="D10" s="388"/>
-      <c r="E10" s="388"/>
-      <c r="F10" s="388"/>
+      <c r="C10" s="399"/>
+      <c r="D10" s="399"/>
+      <c r="E10" s="399"/>
+      <c r="F10" s="399"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
@@ -10095,10 +10095,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="388"/>
-      <c r="D5" s="388"/>
-      <c r="E5" s="388"/>
-      <c r="F5" s="388"/>
+      <c r="C5" s="399"/>
+      <c r="D5" s="399"/>
+      <c r="E5" s="399"/>
+      <c r="F5" s="399"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
         <v>14</v>
@@ -10112,10 +10112,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="388"/>
-      <c r="D6" s="388"/>
-      <c r="E6" s="388"/>
-      <c r="F6" s="388"/>
+      <c r="C6" s="399"/>
+      <c r="D6" s="399"/>
+      <c r="E6" s="399"/>
+      <c r="F6" s="399"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -10159,10 +10159,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="388"/>
-      <c r="D9" s="388"/>
-      <c r="E9" s="388"/>
-      <c r="F9" s="388"/>
+      <c r="C9" s="399"/>
+      <c r="D9" s="399"/>
+      <c r="E9" s="399"/>
+      <c r="F9" s="399"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
@@ -10174,10 +10174,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="388"/>
-      <c r="D10" s="388"/>
-      <c r="E10" s="388"/>
-      <c r="F10" s="388"/>
+      <c r="C10" s="399"/>
+      <c r="D10" s="399"/>
+      <c r="E10" s="399"/>
+      <c r="F10" s="399"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
@@ -10431,11 +10431,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C10:F10"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:I14"/>
     <mergeCell ref="B15:I15"/>
@@ -10443,6 +10438,11 @@
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="B18:I18"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10525,10 +10525,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="388"/>
-      <c r="D5" s="388"/>
-      <c r="E5" s="388"/>
-      <c r="F5" s="388"/>
+      <c r="C5" s="399"/>
+      <c r="D5" s="399"/>
+      <c r="E5" s="399"/>
+      <c r="F5" s="399"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
         <v>14</v>
@@ -10542,10 +10542,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="388"/>
-      <c r="D6" s="388"/>
-      <c r="E6" s="388"/>
-      <c r="F6" s="388"/>
+      <c r="C6" s="399"/>
+      <c r="D6" s="399"/>
+      <c r="E6" s="399"/>
+      <c r="F6" s="399"/>
       <c r="K6" s="56"/>
     </row>
     <row r="7" spans="1:13" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -10585,10 +10585,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="388"/>
-      <c r="D9" s="388"/>
-      <c r="E9" s="388"/>
-      <c r="F9" s="388"/>
+      <c r="C9" s="399"/>
+      <c r="D9" s="399"/>
+      <c r="E9" s="399"/>
+      <c r="F9" s="399"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -10600,10 +10600,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="388"/>
-      <c r="D10" s="388"/>
-      <c r="E10" s="388"/>
-      <c r="F10" s="388"/>
+      <c r="C10" s="399"/>
+      <c r="D10" s="399"/>
+      <c r="E10" s="399"/>
+      <c r="F10" s="399"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -11002,6 +11002,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100570C130F412EDB4EBF3E80DF6A9149FD" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfaa3b10b9be17ef9f56bd19dc71004c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddb0c952b897a810c8a4e377cff6bff8" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -11067,15 +11076,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
   <ds:schemaRefs>
@@ -11085,6 +11085,21 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF64F18F-372D-43EC-AE22-C51BFB121B01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A00BD0D-8423-4FFE-92A4-D273D2078383}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11099,19 +11114,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF64F18F-372D-43EC-AE22-C51BFB121B01}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
individuell klass :  datum,armnr,domare   -  named cells
</commit_message>
<xml_diff>
--- a/mallar/Protokoll 2017 individuell klass_justerat 2017-05-30.xlsx
+++ b/mallar/Protokoll 2017 individuell klass_justerat 2017-05-30.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="PdI6n2wWe1BCLpZSUVKb6Viv2S5eDDxdev/RLVBc6uGkqKIeSnzxpXt+L8Ip+7bcU/gK26fAQjqxcl2KM0Nr6Q==" workbookSaltValue="84UlA07g1xLdi6rLqV4A4w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="10320" windowHeight="7650" tabRatio="941"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="10320" windowHeight="7650" tabRatio="966" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="37" r:id="rId1"/>
@@ -25,6 +25,15 @@
     <sheet name="Individuellt tekniskt artistisk" sheetId="36" r:id="rId10"/>
   </sheets>
   <definedNames>
+    <definedName name="armnr" localSheetId="1">'Häst, individuell'!$L$6</definedName>
+    <definedName name="armnr" localSheetId="5">'Ind kür tekn 1'!$L$7</definedName>
+    <definedName name="armnr" localSheetId="6">'Ind kür tekn 2 3'!$L$7</definedName>
+    <definedName name="armnr" localSheetId="3">'Individuell junior grund 2'!$L$7</definedName>
+    <definedName name="armnr" localSheetId="7">'Individuell kür artistisk'!$L$7</definedName>
+    <definedName name="armnr" localSheetId="2">'Individuell minior grund 1'!$L$7</definedName>
+    <definedName name="armnr" localSheetId="4">'Individuell senior grund 3'!$L$7</definedName>
+    <definedName name="armnr" localSheetId="8">'Individuell tekniska övningar'!$L$7</definedName>
+    <definedName name="armnr" localSheetId="9">'Individuellt tekniskt artistisk'!$L$8</definedName>
     <definedName name="bord" localSheetId="1">'Häst, individuell'!$L$2</definedName>
     <definedName name="bord" localSheetId="5">'Ind kür tekn 1'!$L$3</definedName>
     <definedName name="bord" localSheetId="6">'Ind kür tekn 2 3'!$L$3</definedName>
@@ -34,6 +43,24 @@
     <definedName name="bord" localSheetId="4">'Individuell senior grund 3'!$L$3</definedName>
     <definedName name="bord" localSheetId="8">'Individuell tekniska övningar'!$L$3</definedName>
     <definedName name="bord" localSheetId="9">'Individuellt tekniskt artistisk'!$L$4</definedName>
+    <definedName name="datum" localSheetId="1">'Häst, individuell'!$C$3</definedName>
+    <definedName name="datum" localSheetId="5">'Ind kür tekn 1'!$C$4</definedName>
+    <definedName name="datum" localSheetId="6">'Ind kür tekn 2 3'!$C$4</definedName>
+    <definedName name="datum" localSheetId="3">'Individuell junior grund 2'!$C$4</definedName>
+    <definedName name="datum" localSheetId="7">'Individuell kür artistisk'!$C$4</definedName>
+    <definedName name="datum" localSheetId="2">'Individuell minior grund 1'!$C$4</definedName>
+    <definedName name="datum" localSheetId="4">'Individuell senior grund 3'!$C$4</definedName>
+    <definedName name="datum" localSheetId="8">'Individuell tekniska övningar'!$C$4</definedName>
+    <definedName name="datum" localSheetId="9">'Individuellt tekniskt artistisk'!$C$4</definedName>
+    <definedName name="domare" localSheetId="1">'Häst, individuell'!$C$29</definedName>
+    <definedName name="domare" localSheetId="5">'Ind kür tekn 1'!$C$37</definedName>
+    <definedName name="domare" localSheetId="6">'Ind kür tekn 2 3'!$C$37</definedName>
+    <definedName name="domare" localSheetId="3">'Individuell junior grund 2'!$C$32</definedName>
+    <definedName name="domare" localSheetId="7">'Individuell kür artistisk'!$C$27</definedName>
+    <definedName name="domare" localSheetId="2">'Individuell minior grund 1'!$C$32</definedName>
+    <definedName name="domare" localSheetId="4">'Individuell senior grund 3'!$C$32</definedName>
+    <definedName name="domare" localSheetId="8">'Individuell tekniska övningar'!$C$34</definedName>
+    <definedName name="domare" localSheetId="9">'Individuellt tekniskt artistisk'!$C$28</definedName>
     <definedName name="id" localSheetId="1">'Häst, individuell'!$U$1</definedName>
     <definedName name="id" localSheetId="5">'Ind kür tekn 1'!$U$1</definedName>
     <definedName name="id" localSheetId="6">'Ind kür tekn 2 3'!$U$1</definedName>
@@ -76,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="194">
   <si>
     <t>Nation:</t>
   </si>
@@ -901,9 +928,6 @@
   <si>
     <t>T3
 30%</t>
-  </si>
-  <si>
-    <t>h</t>
   </si>
 </sst>
 </file>
@@ -2838,6 +2862,105 @@
     <xf numFmtId="167" fontId="1" fillId="4" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="173" fontId="2" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="2" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="2" fillId="4" borderId="47" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="2" fillId="4" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="2" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="2" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="46" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="49" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2847,15 +2970,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="47" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2865,102 +2979,12 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="46" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="2" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="2" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="2" fillId="4" borderId="47" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="2" fillId="4" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="2" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="2" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3057,6 +3081,12 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3095,12 +3125,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -3456,7 +3480,7 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:Q84"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="A26" workbookViewId="0">
+    <sheetView showZeros="0" topLeftCell="A26" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -4818,7 +4842,7 @@
   </sheetPr>
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" tabSelected="1" view="pageLayout" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
@@ -5409,17 +5433,17 @@
   <sheetData>
     <row r="1" spans="1:12" s="151" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:12" s="7" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="450" t="s">
+      <c r="A2" s="452" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="450"/>
-      <c r="C2" s="450"/>
-      <c r="D2" s="450"/>
-      <c r="E2" s="450"/>
-      <c r="F2" s="450"/>
-      <c r="G2" s="450"/>
-      <c r="H2" s="450"/>
-      <c r="I2" s="450"/>
+      <c r="B2" s="452"/>
+      <c r="C2" s="452"/>
+      <c r="D2" s="452"/>
+      <c r="E2" s="452"/>
+      <c r="F2" s="452"/>
+      <c r="G2" s="452"/>
+      <c r="H2" s="452"/>
+      <c r="I2" s="452"/>
       <c r="J2" s="186"/>
       <c r="K2" s="186"/>
       <c r="L2" s="186"/>
@@ -5464,10 +5488,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="399"/>
-      <c r="D5" s="399"/>
-      <c r="E5" s="399"/>
-      <c r="F5" s="399"/>
+      <c r="C5" s="388"/>
+      <c r="D5" s="388"/>
+      <c r="E5" s="388"/>
+      <c r="F5" s="388"/>
       <c r="G5" s="185"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
@@ -5482,10 +5506,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="399"/>
-      <c r="D6" s="399"/>
-      <c r="E6" s="399"/>
-      <c r="F6" s="399"/>
+      <c r="C6" s="388"/>
+      <c r="D6" s="388"/>
+      <c r="E6" s="388"/>
+      <c r="F6" s="388"/>
       <c r="G6" s="184"/>
       <c r="H6" s="141"/>
       <c r="I6" s="17" t="s">
@@ -5534,10 +5558,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="399"/>
-      <c r="D9" s="399"/>
-      <c r="E9" s="399"/>
-      <c r="F9" s="399"/>
+      <c r="C9" s="388"/>
+      <c r="D9" s="388"/>
+      <c r="E9" s="388"/>
+      <c r="F9" s="388"/>
       <c r="G9" s="206"/>
       <c r="H9" s="183"/>
       <c r="I9" s="183"/>
@@ -5550,15 +5574,15 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="399"/>
-      <c r="D10" s="399"/>
-      <c r="E10" s="399"/>
-      <c r="F10" s="399"/>
+      <c r="C10" s="388"/>
+      <c r="D10" s="388"/>
+      <c r="E10" s="388"/>
+      <c r="F10" s="388"/>
       <c r="G10" s="206"/>
       <c r="H10" s="183"/>
       <c r="I10" s="183"/>
-      <c r="J10" s="446"/>
-      <c r="K10" s="446"/>
+      <c r="J10" s="448"/>
+      <c r="K10" s="448"/>
       <c r="L10" s="207"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -5585,10 +5609,10 @@
       <c r="C13" s="343" t="s">
         <v>181</v>
       </c>
-      <c r="D13" s="451" t="s">
+      <c r="D13" s="453" t="s">
         <v>182</v>
       </c>
-      <c r="E13" s="452"/>
+      <c r="E13" s="454"/>
       <c r="F13" s="343" t="s">
         <v>183</v>
       </c>
@@ -5601,17 +5625,17 @@
       <c r="I13" s="345" t="s">
         <v>144</v>
       </c>
-      <c r="J13" s="455" t="s">
+      <c r="J13" s="457" t="s">
         <v>190</v>
       </c>
-      <c r="K13" s="456"/>
+      <c r="K13" s="458"/>
       <c r="L13" s="205"/>
     </row>
     <row r="14" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="368"/>
       <c r="C14" s="369"/>
-      <c r="D14" s="453"/>
-      <c r="E14" s="454"/>
+      <c r="D14" s="455"/>
+      <c r="E14" s="456"/>
       <c r="F14" s="369"/>
       <c r="G14" s="369"/>
       <c r="H14" s="370"/>
@@ -5619,11 +5643,11 @@
         <f>SUM(B14:H14)</f>
         <v>0</v>
       </c>
-      <c r="J14" s="457">
+      <c r="J14" s="459">
         <f>I14/6</f>
         <v>0</v>
       </c>
-      <c r="K14" s="458"/>
+      <c r="K14" s="460"/>
       <c r="L14" s="205"/>
     </row>
     <row r="15" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5652,16 +5676,16 @@
       <c r="A17" s="334" t="s">
         <v>189</v>
       </c>
-      <c r="B17" s="447" t="s">
+      <c r="B17" s="449" t="s">
         <v>186</v>
       </c>
-      <c r="C17" s="448"/>
-      <c r="D17" s="448"/>
-      <c r="E17" s="448"/>
-      <c r="F17" s="448"/>
-      <c r="G17" s="448"/>
-      <c r="H17" s="448"/>
-      <c r="I17" s="449"/>
+      <c r="C17" s="450"/>
+      <c r="D17" s="450"/>
+      <c r="E17" s="450"/>
+      <c r="F17" s="450"/>
+      <c r="G17" s="450"/>
+      <c r="H17" s="450"/>
+      <c r="I17" s="451"/>
       <c r="J17" s="203" t="s">
         <v>187</v>
       </c>
@@ -5675,7 +5699,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="459" t="s">
+      <c r="A18" s="446" t="s">
         <v>91</v>
       </c>
       <c r="B18" s="425" t="s">
@@ -5698,7 +5722,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="460"/>
+      <c r="A19" s="447"/>
       <c r="B19" s="427" t="s">
         <v>167</v>
       </c>
@@ -5838,12 +5862,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="A2:I2"/>
@@ -5853,6 +5871,12 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="J14:K14"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5868,8 +5892,8 @@
   <sheetPr codeName="Blad2"/>
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19:K23"/>
+    <sheetView showZeros="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5937,10 +5961,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="14"/>
-      <c r="C4" s="399"/>
-      <c r="D4" s="399"/>
-      <c r="E4" s="399"/>
-      <c r="F4" s="399"/>
+      <c r="C4" s="388"/>
+      <c r="D4" s="388"/>
+      <c r="E4" s="388"/>
+      <c r="F4" s="388"/>
       <c r="H4" s="16"/>
       <c r="I4" s="17" t="s">
         <v>14</v>
@@ -5954,10 +5978,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="399"/>
-      <c r="D5" s="399"/>
-      <c r="E5" s="399"/>
-      <c r="F5" s="399"/>
+      <c r="C5" s="388"/>
+      <c r="D5" s="388"/>
+      <c r="E5" s="388"/>
+      <c r="F5" s="388"/>
       <c r="K5" s="56"/>
     </row>
     <row r="6" spans="1:12" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5982,10 +6006,10 @@
         <v>0</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="399"/>
-      <c r="D7" s="399"/>
-      <c r="E7" s="399"/>
-      <c r="F7" s="399"/>
+      <c r="C7" s="388"/>
+      <c r="D7" s="388"/>
+      <c r="E7" s="388"/>
+      <c r="F7" s="388"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -5997,10 +6021,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="14"/>
-      <c r="C8" s="399"/>
-      <c r="D8" s="399"/>
-      <c r="E8" s="399"/>
-      <c r="F8" s="399"/>
+      <c r="C8" s="388"/>
+      <c r="D8" s="388"/>
+      <c r="E8" s="388"/>
+      <c r="F8" s="388"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -6012,10 +6036,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="399"/>
-      <c r="D9" s="399"/>
-      <c r="E9" s="399"/>
-      <c r="F9" s="399"/>
+      <c r="C9" s="388"/>
+      <c r="D9" s="388"/>
+      <c r="E9" s="388"/>
+      <c r="F9" s="388"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -6049,215 +6073,215 @@
       <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H12" s="400" t="s">
+      <c r="H12" s="389" t="s">
         <v>42</v>
       </c>
-      <c r="I12" s="401"/>
-      <c r="J12" s="402" t="s">
+      <c r="I12" s="390"/>
+      <c r="J12" s="391" t="s">
         <v>43</v>
       </c>
-      <c r="K12" s="402"/>
-      <c r="L12" s="402"/>
+      <c r="K12" s="391"/>
+      <c r="L12" s="391"/>
     </row>
     <row r="13" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="376" t="s">
+      <c r="A13" s="392" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="382" t="s">
+      <c r="B13" s="395" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="382" t="s">
+      <c r="C13" s="395" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="382"/>
-      <c r="E13" s="382"/>
-      <c r="F13" s="391" t="s">
+      <c r="D13" s="395"/>
+      <c r="E13" s="395"/>
+      <c r="F13" s="397" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="392"/>
+      <c r="G13" s="398"/>
       <c r="H13" s="21"/>
       <c r="I13" s="22"/>
-      <c r="J13" s="393" t="s">
+      <c r="J13" s="379" t="s">
         <v>1</v>
       </c>
-      <c r="K13" s="409"/>
-      <c r="L13" s="405">
+      <c r="K13" s="381"/>
+      <c r="L13" s="375">
         <f>ROUND(K13*0.3,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="377"/>
-      <c r="B14" s="387"/>
-      <c r="C14" s="387" t="s">
+      <c r="A14" s="393"/>
+      <c r="B14" s="396"/>
+      <c r="C14" s="396" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="387"/>
-      <c r="E14" s="387"/>
-      <c r="F14" s="388" t="s">
+      <c r="D14" s="396"/>
+      <c r="E14" s="396"/>
+      <c r="F14" s="399" t="s">
         <v>159</v>
       </c>
-      <c r="G14" s="389"/>
+      <c r="G14" s="400"/>
       <c r="H14" s="24"/>
       <c r="I14" s="25"/>
-      <c r="J14" s="394"/>
-      <c r="K14" s="410"/>
-      <c r="L14" s="406"/>
+      <c r="J14" s="380"/>
+      <c r="K14" s="382"/>
+      <c r="L14" s="376"/>
     </row>
     <row r="15" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="377"/>
-      <c r="B15" s="387"/>
-      <c r="C15" s="387" t="s">
+      <c r="A15" s="393"/>
+      <c r="B15" s="396"/>
+      <c r="C15" s="396" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="387"/>
-      <c r="E15" s="387"/>
-      <c r="F15" s="388" t="s">
+      <c r="D15" s="396"/>
+      <c r="E15" s="396"/>
+      <c r="F15" s="399" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="389"/>
+      <c r="G15" s="400"/>
       <c r="H15" s="27"/>
       <c r="I15" s="28"/>
-      <c r="J15" s="394"/>
-      <c r="K15" s="411"/>
-      <c r="L15" s="406"/>
+      <c r="J15" s="380"/>
+      <c r="K15" s="383"/>
+      <c r="L15" s="376"/>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="377"/>
-      <c r="B16" s="395" t="s">
+      <c r="A16" s="393"/>
+      <c r="B16" s="401" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="387" t="s">
+      <c r="C16" s="396" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="387"/>
-      <c r="E16" s="387"/>
-      <c r="F16" s="388" t="s">
+      <c r="D16" s="396"/>
+      <c r="E16" s="396"/>
+      <c r="F16" s="399" t="s">
         <v>160</v>
       </c>
-      <c r="G16" s="389"/>
+      <c r="G16" s="400"/>
       <c r="H16" s="29"/>
       <c r="I16" s="30"/>
-      <c r="J16" s="394" t="s">
+      <c r="J16" s="380" t="s">
         <v>2</v>
       </c>
-      <c r="K16" s="404"/>
-      <c r="L16" s="406">
+      <c r="K16" s="374"/>
+      <c r="L16" s="376">
         <f>ROUND(K16*0.25,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="377"/>
-      <c r="B17" s="396"/>
-      <c r="C17" s="387" t="s">
+      <c r="A17" s="393"/>
+      <c r="B17" s="402"/>
+      <c r="C17" s="396" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="387"/>
-      <c r="E17" s="387"/>
-      <c r="F17" s="388" t="s">
+      <c r="D17" s="396"/>
+      <c r="E17" s="396"/>
+      <c r="F17" s="399" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="389"/>
+      <c r="G17" s="400"/>
       <c r="H17" s="24"/>
       <c r="I17" s="25"/>
-      <c r="J17" s="394"/>
-      <c r="K17" s="404"/>
-      <c r="L17" s="406"/>
+      <c r="J17" s="380"/>
+      <c r="K17" s="374"/>
+      <c r="L17" s="376"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="378"/>
-      <c r="B18" s="397"/>
-      <c r="C18" s="390" t="s">
+      <c r="A18" s="394"/>
+      <c r="B18" s="403"/>
+      <c r="C18" s="405" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="390"/>
-      <c r="E18" s="390"/>
-      <c r="F18" s="385" t="s">
+      <c r="D18" s="405"/>
+      <c r="E18" s="405"/>
+      <c r="F18" s="386" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="386"/>
+      <c r="G18" s="387"/>
       <c r="H18" s="31"/>
       <c r="I18" s="32"/>
-      <c r="J18" s="398"/>
-      <c r="K18" s="412"/>
-      <c r="L18" s="413"/>
+      <c r="J18" s="404"/>
+      <c r="K18" s="384"/>
+      <c r="L18" s="385"/>
     </row>
     <row r="19" spans="1:12" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="376" t="s">
+      <c r="A19" s="392" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="379" t="s">
+      <c r="B19" s="409" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="382" t="s">
+      <c r="C19" s="395" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="382"/>
-      <c r="E19" s="382"/>
-      <c r="F19" s="383" t="s">
+      <c r="D19" s="395"/>
+      <c r="E19" s="395"/>
+      <c r="F19" s="412" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="384"/>
+      <c r="G19" s="413"/>
       <c r="H19" s="33"/>
       <c r="I19" s="34"/>
-      <c r="J19" s="393" t="s">
+      <c r="J19" s="379" t="s">
         <v>104</v>
       </c>
-      <c r="K19" s="403"/>
-      <c r="L19" s="405">
+      <c r="K19" s="373"/>
+      <c r="L19" s="375">
         <f>ROUND(K19*0.25,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="377"/>
-      <c r="B20" s="380"/>
-      <c r="C20" s="387" t="s">
+      <c r="A20" s="393"/>
+      <c r="B20" s="410"/>
+      <c r="C20" s="396" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="387"/>
-      <c r="E20" s="387"/>
-      <c r="F20" s="388" t="s">
+      <c r="D20" s="396"/>
+      <c r="E20" s="396"/>
+      <c r="F20" s="399" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="389"/>
+      <c r="G20" s="400"/>
       <c r="H20" s="24"/>
       <c r="I20" s="25"/>
-      <c r="J20" s="394"/>
-      <c r="K20" s="404"/>
-      <c r="L20" s="406"/>
+      <c r="J20" s="380"/>
+      <c r="K20" s="374"/>
+      <c r="L20" s="376"/>
     </row>
     <row r="21" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="377"/>
-      <c r="B21" s="381"/>
-      <c r="C21" s="387" t="s">
+      <c r="A21" s="393"/>
+      <c r="B21" s="411"/>
+      <c r="C21" s="396" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="387"/>
-      <c r="E21" s="387"/>
-      <c r="F21" s="388" t="s">
+      <c r="D21" s="396"/>
+      <c r="E21" s="396"/>
+      <c r="F21" s="399" t="s">
         <v>34</v>
       </c>
-      <c r="G21" s="389"/>
+      <c r="G21" s="400"/>
       <c r="H21" s="27"/>
       <c r="I21" s="28"/>
-      <c r="J21" s="394"/>
-      <c r="K21" s="404"/>
-      <c r="L21" s="406"/>
+      <c r="J21" s="380"/>
+      <c r="K21" s="374"/>
+      <c r="L21" s="376"/>
     </row>
     <row r="22" spans="1:12" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="378"/>
+      <c r="A22" s="394"/>
       <c r="B22" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="390"/>
-      <c r="D22" s="390"/>
-      <c r="E22" s="390"/>
-      <c r="F22" s="385" t="s">
+      <c r="C22" s="405"/>
+      <c r="D22" s="405"/>
+      <c r="E22" s="405"/>
+      <c r="F22" s="386" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="386"/>
+      <c r="G22" s="387"/>
       <c r="H22" s="36"/>
       <c r="I22" s="37"/>
       <c r="J22" s="38" t="s">
@@ -6276,15 +6300,15 @@
       <c r="B23" s="144" t="s">
         <v>102</v>
       </c>
-      <c r="C23" s="373" t="s">
+      <c r="C23" s="406" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="373"/>
-      <c r="E23" s="373"/>
-      <c r="F23" s="374" t="s">
+      <c r="D23" s="406"/>
+      <c r="E23" s="406"/>
+      <c r="F23" s="407" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="375"/>
+      <c r="G23" s="408"/>
       <c r="H23" s="40"/>
       <c r="I23" s="41"/>
       <c r="J23" s="42" t="s">
@@ -6323,11 +6347,11 @@
         <v>6</v>
       </c>
       <c r="J25" s="46"/>
-      <c r="K25" s="407">
+      <c r="K25" s="377">
         <f>SUM(L13:L23)</f>
         <v>0</v>
       </c>
-      <c r="L25" s="408"/>
+      <c r="L25" s="378"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="K26" s="331"/>
@@ -6354,22 +6378,18 @@
     <row r="30" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="K19:K21"/>
-    <mergeCell ref="L19:L21"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="J19:J21"/>
-    <mergeCell ref="K13:K15"/>
-    <mergeCell ref="L13:L15"/>
-    <mergeCell ref="K16:K18"/>
-    <mergeCell ref="L16:L18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="C22:E22"/>
     <mergeCell ref="A13:A18"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="C13:E13"/>
@@ -6386,18 +6406,22 @@
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="K19:K21"/>
+    <mergeCell ref="L19:L21"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="J19:J21"/>
+    <mergeCell ref="K13:K15"/>
+    <mergeCell ref="L13:L15"/>
+    <mergeCell ref="K16:K18"/>
+    <mergeCell ref="L16:L18"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6413,7 +6437,7 @@
   <sheetPr codeName="Blad3"/>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
@@ -6877,7 +6901,7 @@
   <sheetPr codeName="Blad4"/>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showZeros="0" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
@@ -6945,10 +6969,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="399"/>
-      <c r="D5" s="399"/>
-      <c r="E5" s="399"/>
-      <c r="F5" s="399"/>
+      <c r="C5" s="388"/>
+      <c r="D5" s="388"/>
+      <c r="E5" s="388"/>
+      <c r="F5" s="388"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
         <v>14</v>
@@ -6962,10 +6986,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="399"/>
-      <c r="D6" s="399"/>
-      <c r="E6" s="399"/>
-      <c r="F6" s="399"/>
+      <c r="C6" s="388"/>
+      <c r="D6" s="388"/>
+      <c r="E6" s="388"/>
+      <c r="F6" s="388"/>
       <c r="K6" s="56"/>
     </row>
     <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7005,10 +7029,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="399"/>
-      <c r="D9" s="399"/>
-      <c r="E9" s="399"/>
-      <c r="F9" s="399"/>
+      <c r="C9" s="388"/>
+      <c r="D9" s="388"/>
+      <c r="E9" s="388"/>
+      <c r="F9" s="388"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -7020,10 +7044,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="399"/>
-      <c r="D10" s="399"/>
-      <c r="E10" s="399"/>
-      <c r="F10" s="399"/>
+      <c r="C10" s="388"/>
+      <c r="D10" s="388"/>
+      <c r="E10" s="388"/>
+      <c r="F10" s="388"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -7345,7 +7369,7 @@
   <sheetPr codeName="Blad5"/>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
@@ -7413,10 +7437,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="399"/>
-      <c r="D5" s="399"/>
-      <c r="E5" s="399"/>
-      <c r="F5" s="399"/>
+      <c r="C5" s="388"/>
+      <c r="D5" s="388"/>
+      <c r="E5" s="388"/>
+      <c r="F5" s="388"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
         <v>14</v>
@@ -7430,10 +7454,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="399"/>
-      <c r="D6" s="399"/>
-      <c r="E6" s="399"/>
-      <c r="F6" s="399"/>
+      <c r="C6" s="388"/>
+      <c r="D6" s="388"/>
+      <c r="E6" s="388"/>
+      <c r="F6" s="388"/>
       <c r="K6" s="56"/>
     </row>
     <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7473,10 +7497,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="399"/>
-      <c r="D9" s="399"/>
-      <c r="E9" s="399"/>
-      <c r="F9" s="399"/>
+      <c r="C9" s="388"/>
+      <c r="D9" s="388"/>
+      <c r="E9" s="388"/>
+      <c r="F9" s="388"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -7488,10 +7512,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="399"/>
-      <c r="D10" s="399"/>
-      <c r="E10" s="399"/>
-      <c r="F10" s="399"/>
+      <c r="C10" s="388"/>
+      <c r="D10" s="388"/>
+      <c r="E10" s="388"/>
+      <c r="F10" s="388"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -7812,7 +7836,7 @@
   <sheetPr codeName="Blad6"/>
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
@@ -8309,7 +8333,7 @@
   <sheetPr codeName="Blad7"/>
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
@@ -9007,10 +9031,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="399"/>
-      <c r="D5" s="399"/>
-      <c r="E5" s="399"/>
-      <c r="F5" s="399"/>
+      <c r="C5" s="388"/>
+      <c r="D5" s="388"/>
+      <c r="E5" s="388"/>
+      <c r="F5" s="388"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
         <v>14</v>
@@ -9024,10 +9048,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="399"/>
-      <c r="D6" s="399"/>
-      <c r="E6" s="399"/>
-      <c r="F6" s="399"/>
+      <c r="C6" s="388"/>
+      <c r="D6" s="388"/>
+      <c r="E6" s="388"/>
+      <c r="F6" s="388"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -9071,10 +9095,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="399"/>
-      <c r="D9" s="399"/>
-      <c r="E9" s="399"/>
-      <c r="F9" s="399"/>
+      <c r="C9" s="388"/>
+      <c r="D9" s="388"/>
+      <c r="E9" s="388"/>
+      <c r="F9" s="388"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
@@ -9086,10 +9110,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="399"/>
-      <c r="D10" s="399"/>
-      <c r="E10" s="399"/>
-      <c r="F10" s="399"/>
+      <c r="C10" s="388"/>
+      <c r="D10" s="388"/>
+      <c r="E10" s="388"/>
+      <c r="F10" s="388"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
@@ -9460,8 +9484,8 @@
   <sheetPr codeName="Blad8"/>
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView showZeros="0" topLeftCell="D16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10095,10 +10119,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="399"/>
-      <c r="D5" s="399"/>
-      <c r="E5" s="399"/>
-      <c r="F5" s="399"/>
+      <c r="C5" s="388"/>
+      <c r="D5" s="388"/>
+      <c r="E5" s="388"/>
+      <c r="F5" s="388"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
         <v>14</v>
@@ -10112,10 +10136,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="399"/>
-      <c r="D6" s="399"/>
-      <c r="E6" s="399"/>
-      <c r="F6" s="399"/>
+      <c r="C6" s="388"/>
+      <c r="D6" s="388"/>
+      <c r="E6" s="388"/>
+      <c r="F6" s="388"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -10159,10 +10183,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="399"/>
-      <c r="D9" s="399"/>
-      <c r="E9" s="399"/>
-      <c r="F9" s="399"/>
+      <c r="C9" s="388"/>
+      <c r="D9" s="388"/>
+      <c r="E9" s="388"/>
+      <c r="F9" s="388"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
@@ -10174,10 +10198,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="399"/>
-      <c r="D10" s="399"/>
-      <c r="E10" s="399"/>
-      <c r="F10" s="399"/>
+      <c r="C10" s="388"/>
+      <c r="D10" s="388"/>
+      <c r="E10" s="388"/>
+      <c r="F10" s="388"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
@@ -10382,11 +10406,7 @@
     </row>
     <row r="24" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E26" s="7" t="s">
-        <v>194</v>
-      </c>
-    </row>
+    <row r="26" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>44</v>
@@ -10431,6 +10451,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C10:F10"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:I14"/>
     <mergeCell ref="B15:I15"/>
@@ -10438,11 +10463,6 @@
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="B18:I18"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10460,7 +10480,7 @@
   </sheetPr>
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -10525,10 +10545,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="399"/>
-      <c r="D5" s="399"/>
-      <c r="E5" s="399"/>
-      <c r="F5" s="399"/>
+      <c r="C5" s="388"/>
+      <c r="D5" s="388"/>
+      <c r="E5" s="388"/>
+      <c r="F5" s="388"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
         <v>14</v>
@@ -10542,10 +10562,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="399"/>
-      <c r="D6" s="399"/>
-      <c r="E6" s="399"/>
-      <c r="F6" s="399"/>
+      <c r="C6" s="388"/>
+      <c r="D6" s="388"/>
+      <c r="E6" s="388"/>
+      <c r="F6" s="388"/>
       <c r="K6" s="56"/>
     </row>
     <row r="7" spans="1:13" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -10585,10 +10605,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="399"/>
-      <c r="D9" s="399"/>
-      <c r="E9" s="399"/>
-      <c r="F9" s="399"/>
+      <c r="C9" s="388"/>
+      <c r="D9" s="388"/>
+      <c r="E9" s="388"/>
+      <c r="F9" s="388"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -10600,10 +10620,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="399"/>
-      <c r="D10" s="399"/>
-      <c r="E10" s="399"/>
-      <c r="F10" s="399"/>
+      <c r="C10" s="388"/>
+      <c r="D10" s="388"/>
+      <c r="E10" s="388"/>
+      <c r="F10" s="388"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -11002,15 +11022,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100570C130F412EDB4EBF3E80DF6A9149FD" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfaa3b10b9be17ef9f56bd19dc71004c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddb0c952b897a810c8a4e377cff6bff8" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -11076,6 +11087,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
   <ds:schemaRefs>
@@ -11085,21 +11105,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF64F18F-372D-43EC-AE22-C51BFB121B01}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A00BD0D-8423-4FFE-92A4-D273D2078383}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11114,4 +11119,19 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF64F18F-372D-43EC-AE22-C51BFB121B01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Visa logg på vad som ändras vid inport
</commit_message>
<xml_diff>
--- a/mallar/Protokoll 2017 individuell klass_justerat 2017-05-30.xlsx
+++ b/mallar/Protokoll 2017 individuell klass_justerat 2017-05-30.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magnus.sandberg\Documents\Visual Studio 2015\Projects\VoltigeClosedXML\mallar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6025D8-81CB-4B36-9DA7-0569EF69B11E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3EA182-F109-432D-860A-848413F674E6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="PdI6n2wWe1BCLpZSUVKb6Viv2S5eDDxdev/RLVBc6uGkqKIeSnzxpXt+L8Ip+7bcU/gK26fAQjqxcl2KM0Nr6Q==" workbookSaltValue="84UlA07g1xLdi6rLqV4A4w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="10320" windowHeight="7650" tabRatio="966" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="10320" windowHeight="7650" tabRatio="966" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="37" r:id="rId1"/>
@@ -99,12 +99,12 @@
     <definedName name="result" localSheetId="8">'Individuell tekniska övningar'!$L$30</definedName>
     <definedName name="result" localSheetId="9">'Individuellt tekniskt artistisk'!$L$24</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="192">
   <si>
     <t>Nation:</t>
   </si>
@@ -333,18 +333,6 @@
   </si>
   <si>
     <t>Sidhopp del 1</t>
-  </si>
-  <si>
-    <t>Grundövningar 3*</t>
-  </si>
-  <si>
-    <t>Grundövningar 2*</t>
-  </si>
-  <si>
-    <t>Grundövningar 1*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Individuell minior 1* </t>
   </si>
   <si>
     <t>Teknisk bedömning</t>
@@ -928,6 +916,12 @@
 • Stor variation av uttryck som speglar olika typer av musik samt förändringar i musiken
 • Komplext kroppsspråk samt gester och rörelser i många olika riktningar.</t>
     </r>
+  </si>
+  <si>
+    <t>Grundövningar</t>
+  </si>
+  <si>
+    <t>Individuell minior</t>
   </si>
 </sst>
 </file>
@@ -2869,6 +2863,105 @@
     <xf numFmtId="167" fontId="1" fillId="4" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="173" fontId="2" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="2" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="2" fillId="4" borderId="47" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="2" fillId="4" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="2" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="2" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="46" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="49" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2878,15 +2971,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="47" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2896,102 +2980,12 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="27" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="46" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="2" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="2" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="2" fillId="4" borderId="47" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="2" fillId="4" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="2" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="2" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3016,6 +3010,9 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
@@ -3085,6 +3082,12 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3123,15 +3126,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -3499,34 +3493,34 @@
   <sheetData>
     <row r="1" spans="1:8" s="320" customFormat="1" ht="20.65" x14ac:dyDescent="0.6">
       <c r="A1" s="319" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="320" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="320" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="320" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="320" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="320" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:8" s="320" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="320" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="320" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:8" s="283" customFormat="1" ht="17.25" x14ac:dyDescent="0.45">
       <c r="A7" s="283" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="208" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -3534,61 +3528,61 @@
     </row>
     <row r="11" spans="1:8" s="284" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A11" s="284" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="285" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C12" s="208"/>
       <c r="F12" s="285" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="284" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C13" s="284" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D13" s="284" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E13" s="284"/>
       <c r="F13" s="284" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G13" s="284" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H13" s="284" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="208" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B14" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C14" s="280" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D14" s="280" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E14" s="287"/>
       <c r="F14" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G14" s="280" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H14" s="280" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -3603,26 +3597,26 @@
     </row>
     <row r="16" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="208" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B16" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C16" s="280" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D16" s="280" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E16" s="287"/>
       <c r="F16" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G16" s="280" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H16" s="280" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -3637,26 +3631,26 @@
     </row>
     <row r="18" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="208" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B18" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C18" s="280" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D18" s="280" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E18" s="287"/>
       <c r="F18" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G18" s="280" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H18" s="280" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -3671,40 +3665,40 @@
     </row>
     <row r="20" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="208" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B20" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C20" s="280" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D20" s="280" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E20" s="287"/>
       <c r="F20" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G20" s="280" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H20" s="280" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A21" s="333" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B21" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C21" s="280" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D21" s="280" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E21" s="286"/>
     </row>
@@ -3717,110 +3711,110 @@
     </row>
     <row r="23" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="208" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B23" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C23" s="280" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D23" s="280" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E23" s="287"/>
       <c r="F23" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G23" s="280" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H23" s="280" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A24" s="333" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B24" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C24" s="280" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D24" s="280" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E24" s="286"/>
     </row>
     <row r="26" spans="1:9" s="284" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A26" s="284" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="285" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C27" s="208"/>
       <c r="F27" s="285" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B28" s="284" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C28" s="284" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D28" s="284" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E28" s="284" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F28" s="284" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G28" s="284" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H28" s="284" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I28" s="284" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="208" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B29" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C29" s="280" t="s">
+        <v>121</v>
+      </c>
+      <c r="D29" s="280" t="s">
+        <v>121</v>
+      </c>
+      <c r="E29" s="280" t="s">
+        <v>121</v>
+      </c>
+      <c r="F29" s="280" t="s">
+        <v>124</v>
+      </c>
+      <c r="G29" s="280" t="s">
         <v>125</v>
       </c>
-      <c r="D29" s="280" t="s">
+      <c r="H29" s="280" t="s">
+        <v>127</v>
+      </c>
+      <c r="I29" s="280" t="s">
         <v>125</v>
-      </c>
-      <c r="E29" s="280" t="s">
-        <v>125</v>
-      </c>
-      <c r="F29" s="280" t="s">
-        <v>128</v>
-      </c>
-      <c r="G29" s="280" t="s">
-        <v>129</v>
-      </c>
-      <c r="H29" s="280" t="s">
-        <v>131</v>
-      </c>
-      <c r="I29" s="280" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -3836,31 +3830,31 @@
     </row>
     <row r="31" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="208" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B31" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C31" s="280" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" s="280" t="s">
+        <v>122</v>
+      </c>
+      <c r="E31" s="280" t="s">
+        <v>122</v>
+      </c>
+      <c r="F31" s="280" t="s">
+        <v>124</v>
+      </c>
+      <c r="G31" s="280" t="s">
         <v>126</v>
       </c>
-      <c r="D31" s="280" t="s">
+      <c r="H31" s="280" t="s">
+        <v>127</v>
+      </c>
+      <c r="I31" s="280" t="s">
         <v>126</v>
-      </c>
-      <c r="E31" s="280" t="s">
-        <v>126</v>
-      </c>
-      <c r="F31" s="280" t="s">
-        <v>128</v>
-      </c>
-      <c r="G31" s="280" t="s">
-        <v>130</v>
-      </c>
-      <c r="H31" s="280" t="s">
-        <v>131</v>
-      </c>
-      <c r="I31" s="280" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -3876,31 +3870,31 @@
     </row>
     <row r="33" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="208" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B33" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C33" s="280" t="s">
+        <v>123</v>
+      </c>
+      <c r="D33" s="280" t="s">
+        <v>123</v>
+      </c>
+      <c r="E33" s="280" t="s">
+        <v>123</v>
+      </c>
+      <c r="F33" s="280" t="s">
+        <v>124</v>
+      </c>
+      <c r="G33" s="280" t="s">
+        <v>126</v>
+      </c>
+      <c r="H33" s="280" t="s">
         <v>127</v>
       </c>
-      <c r="D33" s="280" t="s">
-        <v>127</v>
-      </c>
-      <c r="E33" s="280" t="s">
-        <v>127</v>
-      </c>
-      <c r="F33" s="280" t="s">
-        <v>128</v>
-      </c>
-      <c r="G33" s="280" t="s">
-        <v>130</v>
-      </c>
-      <c r="H33" s="280" t="s">
-        <v>131</v>
-      </c>
       <c r="I33" s="280" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -3916,48 +3910,48 @@
     </row>
     <row r="35" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="208" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B35" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C35" s="280" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D35" s="280" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E35" s="280" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F35" s="282" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G35" s="280" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H35" s="280" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="I35" s="280" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A36" s="333" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B36" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C36" s="280" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D36" s="280" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E36" s="280" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.35">
@@ -3968,48 +3962,48 @@
     </row>
     <row r="38" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="208" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B38" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C38" s="280" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" s="280" t="s">
+        <v>123</v>
+      </c>
+      <c r="E38" s="280" t="s">
+        <v>123</v>
+      </c>
+      <c r="F38" s="280" t="s">
+        <v>124</v>
+      </c>
+      <c r="G38" s="280" t="s">
+        <v>126</v>
+      </c>
+      <c r="H38" s="280" t="s">
         <v>127</v>
       </c>
-      <c r="D38" s="280" t="s">
-        <v>127</v>
-      </c>
-      <c r="E38" s="280" t="s">
-        <v>127</v>
-      </c>
-      <c r="F38" s="280" t="s">
-        <v>128</v>
-      </c>
-      <c r="G38" s="280" t="s">
-        <v>130</v>
-      </c>
-      <c r="H38" s="280" t="s">
-        <v>131</v>
-      </c>
       <c r="I38" s="280" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A39" s="333" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B39" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C39" s="280" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D39" s="280" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E39" s="280" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.35">
@@ -4026,106 +4020,106 @@
     </row>
     <row r="42" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A42" s="284" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B44" s="285" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C44" s="208"/>
       <c r="F44" s="285" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="J44" s="285" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="K44" s="208"/>
       <c r="N44" s="285" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B45" s="284" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C45" s="284" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D45" s="284" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E45" s="284"/>
       <c r="F45" s="284" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G45" s="284" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H45" s="284" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="J45" s="284" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K45" s="284" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L45" s="284" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="M45" s="284"/>
       <c r="N45" s="284" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="O45" s="284" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="P45" s="284" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="208" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B46" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C46" s="280" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D46" s="280" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E46" s="287"/>
       <c r="F46" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G46" s="280" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H46" s="280" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="J46" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="K46" s="280" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="L46" s="280" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="M46" s="287"/>
       <c r="N46" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="O46" s="280" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="P46" s="280" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -4147,45 +4141,45 @@
     </row>
     <row r="48" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="208" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B48" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C48" s="280" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D48" s="280" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E48" s="287"/>
       <c r="F48" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G48" s="280" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H48" s="280" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="J48" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="K48" s="280" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="L48" s="280" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="M48" s="287"/>
       <c r="N48" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="O48" s="280" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="P48" s="280" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -4207,45 +4201,45 @@
     </row>
     <row r="50" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="208" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B50" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C50" s="280" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D50" s="280" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E50" s="287"/>
       <c r="F50" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G50" s="280" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H50" s="280" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="J50" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="K50" s="280" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="L50" s="280" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="M50" s="287"/>
       <c r="N50" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="O50" s="280" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="P50" s="280" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -4267,45 +4261,45 @@
     </row>
     <row r="52" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="208" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B52" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C52" s="280" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D52" s="280" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E52" s="287"/>
       <c r="F52" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G52" s="280" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H52" s="280" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J52" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="K52" s="280" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="L52" s="280" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="M52" s="287"/>
       <c r="N52" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="O52" s="280" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="P52" s="280" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.35">
@@ -4317,126 +4311,126 @@
     </row>
     <row r="55" spans="1:17" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A55" s="284" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="57" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B57" s="285" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C57" s="208"/>
       <c r="F57" s="285" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="J57" s="285" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="K57" s="208"/>
       <c r="N57" s="285" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B58" s="284" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C58" s="284" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D58" s="284" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E58" s="284" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F58" s="284" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G58" s="284" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H58" s="284" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I58" s="284" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="J58" s="284" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K58" s="284" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L58" s="284" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="M58" s="284" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="N58" s="284" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="O58" s="284" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="P58" s="284" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="Q58" s="284" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="59" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="208" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B59" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C59" s="280" t="s">
+        <v>121</v>
+      </c>
+      <c r="D59" s="280" t="s">
+        <v>121</v>
+      </c>
+      <c r="E59" s="280" t="s">
+        <v>121</v>
+      </c>
+      <c r="F59" s="280" t="s">
+        <v>124</v>
+      </c>
+      <c r="G59" s="280" t="s">
         <v>125</v>
       </c>
-      <c r="D59" s="280" t="s">
+      <c r="H59" s="280" t="s">
+        <v>127</v>
+      </c>
+      <c r="I59" s="280" t="s">
         <v>125</v>
       </c>
-      <c r="E59" s="280" t="s">
+      <c r="J59" s="280" t="s">
+        <v>124</v>
+      </c>
+      <c r="K59" s="280" t="s">
+        <v>121</v>
+      </c>
+      <c r="L59" s="280" t="s">
+        <v>121</v>
+      </c>
+      <c r="M59" s="280" t="s">
+        <v>121</v>
+      </c>
+      <c r="N59" s="280" t="s">
+        <v>124</v>
+      </c>
+      <c r="O59" s="280" t="s">
         <v>125</v>
       </c>
-      <c r="F59" s="280" t="s">
-        <v>128</v>
-      </c>
-      <c r="G59" s="280" t="s">
-        <v>129</v>
-      </c>
-      <c r="H59" s="280" t="s">
-        <v>131</v>
-      </c>
-      <c r="I59" s="280" t="s">
-        <v>129</v>
-      </c>
-      <c r="J59" s="280" t="s">
-        <v>128</v>
-      </c>
-      <c r="K59" s="280" t="s">
+      <c r="P59" s="280" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q59" s="280" t="s">
         <v>125</v>
-      </c>
-      <c r="L59" s="280" t="s">
-        <v>125</v>
-      </c>
-      <c r="M59" s="280" t="s">
-        <v>125</v>
-      </c>
-      <c r="N59" s="280" t="s">
-        <v>128</v>
-      </c>
-      <c r="O59" s="280" t="s">
-        <v>129</v>
-      </c>
-      <c r="P59" s="280" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q59" s="280" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -4460,55 +4454,55 @@
     </row>
     <row r="61" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="208" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B61" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C61" s="280" t="s">
+        <v>122</v>
+      </c>
+      <c r="D61" s="280" t="s">
+        <v>122</v>
+      </c>
+      <c r="E61" s="280" t="s">
+        <v>122</v>
+      </c>
+      <c r="F61" s="280" t="s">
+        <v>124</v>
+      </c>
+      <c r="G61" s="280" t="s">
         <v>126</v>
       </c>
-      <c r="D61" s="280" t="s">
+      <c r="H61" s="280" t="s">
+        <v>127</v>
+      </c>
+      <c r="I61" s="280" t="s">
         <v>126</v>
       </c>
-      <c r="E61" s="280" t="s">
+      <c r="J61" s="280" t="s">
+        <v>124</v>
+      </c>
+      <c r="K61" s="280" t="s">
+        <v>122</v>
+      </c>
+      <c r="L61" s="280" t="s">
+        <v>122</v>
+      </c>
+      <c r="M61" s="280" t="s">
+        <v>122</v>
+      </c>
+      <c r="N61" s="280" t="s">
+        <v>124</v>
+      </c>
+      <c r="O61" s="280" t="s">
         <v>126</v>
       </c>
-      <c r="F61" s="280" t="s">
-        <v>128</v>
-      </c>
-      <c r="G61" s="280" t="s">
-        <v>130</v>
-      </c>
-      <c r="H61" s="280" t="s">
-        <v>131</v>
-      </c>
-      <c r="I61" s="280" t="s">
-        <v>130</v>
-      </c>
-      <c r="J61" s="280" t="s">
-        <v>128</v>
-      </c>
-      <c r="K61" s="280" t="s">
+      <c r="P61" s="280" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q61" s="280" t="s">
         <v>126</v>
-      </c>
-      <c r="L61" s="280" t="s">
-        <v>126</v>
-      </c>
-      <c r="M61" s="280" t="s">
-        <v>126</v>
-      </c>
-      <c r="N61" s="280" t="s">
-        <v>128</v>
-      </c>
-      <c r="O61" s="280" t="s">
-        <v>130</v>
-      </c>
-      <c r="P61" s="280" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q61" s="280" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -4532,55 +4526,55 @@
     </row>
     <row r="63" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="208" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B63" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C63" s="280" t="s">
+        <v>123</v>
+      </c>
+      <c r="D63" s="280" t="s">
+        <v>123</v>
+      </c>
+      <c r="E63" s="280" t="s">
+        <v>123</v>
+      </c>
+      <c r="F63" s="280" t="s">
+        <v>124</v>
+      </c>
+      <c r="G63" s="280" t="s">
+        <v>126</v>
+      </c>
+      <c r="H63" s="280" t="s">
         <v>127</v>
       </c>
-      <c r="D63" s="280" t="s">
+      <c r="I63" s="280" t="s">
+        <v>126</v>
+      </c>
+      <c r="J63" s="280" t="s">
+        <v>124</v>
+      </c>
+      <c r="K63" s="280" t="s">
+        <v>123</v>
+      </c>
+      <c r="L63" s="280" t="s">
+        <v>123</v>
+      </c>
+      <c r="M63" s="280" t="s">
+        <v>123</v>
+      </c>
+      <c r="N63" s="280" t="s">
+        <v>124</v>
+      </c>
+      <c r="O63" s="280" t="s">
+        <v>126</v>
+      </c>
+      <c r="P63" s="280" t="s">
         <v>127</v>
       </c>
-      <c r="E63" s="280" t="s">
-        <v>127</v>
-      </c>
-      <c r="F63" s="280" t="s">
-        <v>128</v>
-      </c>
-      <c r="G63" s="280" t="s">
-        <v>130</v>
-      </c>
-      <c r="H63" s="280" t="s">
-        <v>131</v>
-      </c>
-      <c r="I63" s="280" t="s">
-        <v>130</v>
-      </c>
-      <c r="J63" s="280" t="s">
-        <v>128</v>
-      </c>
-      <c r="K63" s="280" t="s">
-        <v>127</v>
-      </c>
-      <c r="L63" s="280" t="s">
-        <v>127</v>
-      </c>
-      <c r="M63" s="280" t="s">
-        <v>127</v>
-      </c>
-      <c r="N63" s="280" t="s">
-        <v>128</v>
-      </c>
-      <c r="O63" s="280" t="s">
-        <v>130</v>
-      </c>
-      <c r="P63" s="280" t="s">
-        <v>131</v>
-      </c>
       <c r="Q63" s="280" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -4604,60 +4598,60 @@
     </row>
     <row r="65" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="208" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B65" s="280" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C65" s="280" t="s">
+        <v>123</v>
+      </c>
+      <c r="D65" s="280" t="s">
+        <v>123</v>
+      </c>
+      <c r="E65" s="280" t="s">
+        <v>123</v>
+      </c>
+      <c r="F65" s="280" t="s">
+        <v>124</v>
+      </c>
+      <c r="G65" s="280" t="s">
+        <v>130</v>
+      </c>
+      <c r="H65" s="280" t="s">
+        <v>131</v>
+      </c>
+      <c r="I65" s="280" t="s">
+        <v>130</v>
+      </c>
+      <c r="J65" s="280" t="s">
+        <v>124</v>
+      </c>
+      <c r="K65" s="280" t="s">
+        <v>126</v>
+      </c>
+      <c r="L65" s="280" t="s">
         <v>127</v>
       </c>
-      <c r="D65" s="280" t="s">
-        <v>127</v>
-      </c>
-      <c r="E65" s="280" t="s">
-        <v>127</v>
-      </c>
-      <c r="F65" s="280" t="s">
-        <v>128</v>
-      </c>
-      <c r="G65" s="280" t="s">
-        <v>134</v>
-      </c>
-      <c r="H65" s="280" t="s">
-        <v>135</v>
-      </c>
-      <c r="I65" s="280" t="s">
-        <v>134</v>
-      </c>
-      <c r="J65" s="280" t="s">
-        <v>128</v>
-      </c>
-      <c r="K65" s="280" t="s">
+      <c r="M65" s="280" t="s">
+        <v>126</v>
+      </c>
+      <c r="N65" s="280" t="s">
+        <v>124</v>
+      </c>
+      <c r="O65" s="280" t="s">
         <v>130</v>
       </c>
-      <c r="L65" s="280" t="s">
+      <c r="P65" s="280" t="s">
         <v>131</v>
       </c>
-      <c r="M65" s="280" t="s">
+      <c r="Q65" s="280" t="s">
         <v>130</v>
-      </c>
-      <c r="N65" s="280" t="s">
-        <v>128</v>
-      </c>
-      <c r="O65" s="280" t="s">
-        <v>134</v>
-      </c>
-      <c r="P65" s="280" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q65" s="280" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="69" spans="1:17" s="323" customFormat="1" ht="17.25" x14ac:dyDescent="0.45">
       <c r="A69" s="322" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="70" spans="1:17" s="284" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
@@ -4665,79 +4659,79 @@
         <v>66</v>
       </c>
       <c r="B70" s="327" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C70" s="327" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D70" s="327" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E70" s="327" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F70" s="327" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="321" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B71" s="321" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C71" s="329" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D71" s="329" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E71" s="321" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F71" s="321" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="321" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B72" s="321" t="s">
+        <v>142</v>
+      </c>
+      <c r="C72" s="321" t="s">
         <v>146</v>
       </c>
-      <c r="C72" s="321" t="s">
-        <v>150</v>
-      </c>
       <c r="D72" s="321" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E72" s="321" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F72" s="321" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="321" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B73" s="321" t="s">
+        <v>142</v>
+      </c>
+      <c r="C73" s="321" t="s">
         <v>146</v>
       </c>
-      <c r="C73" s="321" t="s">
-        <v>150</v>
-      </c>
       <c r="D73" s="321" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E73" s="321" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F73" s="321" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="74" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4747,7 +4741,7 @@
       <c r="D74" s="321"/>
       <c r="E74" s="321"/>
       <c r="F74" s="324" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="75" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4768,62 +4762,62 @@
     </row>
     <row r="78" spans="1:17" s="284" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A78" s="328" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B78" s="327" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C78" s="327" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D78" s="327" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E78" s="327" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F78" s="327" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" s="321" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B79" s="321" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C79" s="329" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D79" s="329" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E79" s="321" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F79" s="321" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A80" s="321" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B80" s="321" t="s">
+        <v>142</v>
+      </c>
+      <c r="C80" s="321" t="s">
         <v>146</v>
       </c>
-      <c r="C80" s="321" t="s">
-        <v>150</v>
-      </c>
       <c r="D80" s="321" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E80" s="321" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F80" s="321" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4833,7 +4827,7 @@
       <c r="D81" s="321"/>
       <c r="E81" s="321"/>
       <c r="F81" s="280" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="84" spans="1:6" s="322" customFormat="1" ht="17.25" x14ac:dyDescent="0.45"/>
@@ -4849,7 +4843,7 @@
   </sheetPr>
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
@@ -5440,24 +5434,24 @@
   <sheetData>
     <row r="1" spans="1:12" s="151" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:12" s="7" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="449" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="449"/>
-      <c r="C2" s="449"/>
-      <c r="D2" s="449"/>
-      <c r="E2" s="449"/>
-      <c r="F2" s="449"/>
-      <c r="G2" s="449"/>
-      <c r="H2" s="449"/>
-      <c r="I2" s="449"/>
+      <c r="A2" s="452" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="452"/>
+      <c r="C2" s="452"/>
+      <c r="D2" s="452"/>
+      <c r="E2" s="452"/>
+      <c r="F2" s="452"/>
+      <c r="G2" s="452"/>
+      <c r="H2" s="452"/>
+      <c r="I2" s="452"/>
       <c r="J2" s="186"/>
       <c r="K2" s="186"/>
       <c r="L2" s="186"/>
     </row>
     <row r="3" spans="1:12" s="151" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -5466,7 +5460,7 @@
       <c r="F3" s="1"/>
       <c r="H3" s="141"/>
       <c r="I3" s="17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J3" s="18"/>
       <c r="K3" s="142"/>
@@ -5484,7 +5478,7 @@
       <c r="G4" s="185"/>
       <c r="H4" s="141"/>
       <c r="I4" s="17" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J4" s="18"/>
       <c r="K4" s="142"/>
@@ -5495,10 +5489,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="399"/>
-      <c r="D5" s="399"/>
-      <c r="E5" s="399"/>
-      <c r="F5" s="399"/>
+      <c r="C5" s="388"/>
+      <c r="D5" s="388"/>
+      <c r="E5" s="388"/>
+      <c r="F5" s="388"/>
       <c r="G5" s="185"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
@@ -5513,10 +5507,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="399"/>
-      <c r="D6" s="399"/>
-      <c r="E6" s="399"/>
-      <c r="F6" s="399"/>
+      <c r="C6" s="388"/>
+      <c r="D6" s="388"/>
+      <c r="E6" s="388"/>
+      <c r="F6" s="388"/>
       <c r="G6" s="184"/>
       <c r="H6" s="141"/>
       <c r="I6" s="17" t="s">
@@ -5565,10 +5559,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="399"/>
-      <c r="D9" s="399"/>
-      <c r="E9" s="399"/>
-      <c r="F9" s="399"/>
+      <c r="C9" s="388"/>
+      <c r="D9" s="388"/>
+      <c r="E9" s="388"/>
+      <c r="F9" s="388"/>
       <c r="G9" s="206"/>
       <c r="H9" s="183"/>
       <c r="I9" s="183"/>
@@ -5581,15 +5575,15 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="399"/>
-      <c r="D10" s="399"/>
-      <c r="E10" s="399"/>
-      <c r="F10" s="399"/>
+      <c r="C10" s="388"/>
+      <c r="D10" s="388"/>
+      <c r="E10" s="388"/>
+      <c r="F10" s="388"/>
       <c r="G10" s="206"/>
       <c r="H10" s="183"/>
       <c r="I10" s="183"/>
-      <c r="J10" s="445"/>
-      <c r="K10" s="445"/>
+      <c r="J10" s="448"/>
+      <c r="K10" s="448"/>
       <c r="L10" s="207"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -5601,7 +5595,7 @@
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="158" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="H12" s="205"/>
       <c r="I12" s="205"/>
@@ -5611,38 +5605,38 @@
     </row>
     <row r="13" spans="1:12" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="342" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" s="343" t="s">
+        <v>176</v>
+      </c>
+      <c r="D13" s="453" t="s">
+        <v>177</v>
+      </c>
+      <c r="E13" s="454"/>
+      <c r="F13" s="343" t="s">
+        <v>178</v>
+      </c>
+      <c r="G13" s="343" t="s">
         <v>179</v>
       </c>
-      <c r="C13" s="343" t="s">
+      <c r="H13" s="344" t="s">
         <v>180</v>
       </c>
-      <c r="D13" s="450" t="s">
-        <v>181</v>
-      </c>
-      <c r="E13" s="451"/>
-      <c r="F13" s="343" t="s">
-        <v>182</v>
-      </c>
-      <c r="G13" s="343" t="s">
-        <v>183</v>
-      </c>
-      <c r="H13" s="344" t="s">
-        <v>184</v>
-      </c>
       <c r="I13" s="345" t="s">
-        <v>144</v>
-      </c>
-      <c r="J13" s="454" t="s">
-        <v>189</v>
-      </c>
-      <c r="K13" s="455"/>
+        <v>140</v>
+      </c>
+      <c r="J13" s="457" t="s">
+        <v>185</v>
+      </c>
+      <c r="K13" s="458"/>
       <c r="L13" s="205"/>
     </row>
     <row r="14" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="368"/>
       <c r="C14" s="369"/>
-      <c r="D14" s="452"/>
-      <c r="E14" s="453"/>
+      <c r="D14" s="455"/>
+      <c r="E14" s="456"/>
       <c r="F14" s="369"/>
       <c r="G14" s="369"/>
       <c r="H14" s="370"/>
@@ -5650,11 +5644,11 @@
         <f>SUM(B14:H14)</f>
         <v>0</v>
       </c>
-      <c r="J14" s="456">
+      <c r="J14" s="459">
         <f>I14/6</f>
         <v>0</v>
       </c>
-      <c r="K14" s="457"/>
+      <c r="K14" s="460"/>
       <c r="L14" s="205"/>
     </row>
     <row r="15" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5675,26 +5669,26 @@
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="341" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="L16" s="12"/>
     </row>
     <row r="17" spans="1:12" ht="61.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="334" t="s">
-        <v>188</v>
-      </c>
-      <c r="B17" s="446" t="s">
-        <v>185</v>
-      </c>
-      <c r="C17" s="447"/>
-      <c r="D17" s="447"/>
-      <c r="E17" s="447"/>
-      <c r="F17" s="447"/>
-      <c r="G17" s="447"/>
-      <c r="H17" s="447"/>
-      <c r="I17" s="448"/>
+        <v>184</v>
+      </c>
+      <c r="B17" s="449" t="s">
+        <v>181</v>
+      </c>
+      <c r="C17" s="450"/>
+      <c r="D17" s="450"/>
+      <c r="E17" s="450"/>
+      <c r="F17" s="450"/>
+      <c r="G17" s="450"/>
+      <c r="H17" s="450"/>
+      <c r="I17" s="451"/>
       <c r="J17" s="203" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="K17" s="315">
         <f>J14</f>
@@ -5706,21 +5700,21 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="458" t="s">
-        <v>91</v>
-      </c>
-      <c r="B18" s="424" t="s">
+      <c r="A18" s="446" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="425" t="s">
+        <v>183</v>
+      </c>
+      <c r="C18" s="426"/>
+      <c r="D18" s="426"/>
+      <c r="E18" s="426"/>
+      <c r="F18" s="426"/>
+      <c r="G18" s="426"/>
+      <c r="H18" s="426"/>
+      <c r="I18" s="426"/>
+      <c r="J18" s="203" t="s">
         <v>187</v>
-      </c>
-      <c r="C18" s="425"/>
-      <c r="D18" s="425"/>
-      <c r="E18" s="425"/>
-      <c r="F18" s="425"/>
-      <c r="G18" s="425"/>
-      <c r="H18" s="425"/>
-      <c r="I18" s="425"/>
-      <c r="J18" s="203" t="s">
-        <v>191</v>
       </c>
       <c r="K18" s="363"/>
       <c r="L18" s="202">
@@ -5729,19 +5723,19 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="459"/>
-      <c r="B19" s="426" t="s">
-        <v>166</v>
-      </c>
-      <c r="C19" s="427"/>
-      <c r="D19" s="427"/>
-      <c r="E19" s="427"/>
-      <c r="F19" s="427"/>
-      <c r="G19" s="427"/>
-      <c r="H19" s="427"/>
-      <c r="I19" s="427"/>
+      <c r="A19" s="447"/>
+      <c r="B19" s="427" t="s">
+        <v>162</v>
+      </c>
+      <c r="C19" s="428"/>
+      <c r="D19" s="428"/>
+      <c r="E19" s="428"/>
+      <c r="F19" s="428"/>
+      <c r="G19" s="428"/>
+      <c r="H19" s="428"/>
+      <c r="I19" s="428"/>
       <c r="J19" s="201" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="K19" s="364"/>
       <c r="L19" s="200">
@@ -5783,7 +5777,7 @@
     <row r="22" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="171"/>
       <c r="B22" s="198" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C22" s="197"/>
       <c r="D22" s="196"/>
@@ -5799,7 +5793,7 @@
     <row r="23" spans="1:12" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I24" s="195" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J24" s="194"/>
       <c r="K24" s="194"/>
@@ -5869,12 +5863,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="A2:I2"/>
@@ -5884,6 +5872,12 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="J14:K14"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5899,7 +5893,7 @@
   <sheetPr codeName="Blad2"/>
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -5928,7 +5922,7 @@
       <c r="F1" s="132"/>
       <c r="H1" s="141"/>
       <c r="I1" s="17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J1" s="18"/>
       <c r="K1" s="142"/>
@@ -5940,7 +5934,7 @@
       </c>
       <c r="H2" s="141"/>
       <c r="I2" s="17" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J2" s="18"/>
       <c r="K2" s="142"/>
@@ -5968,10 +5962,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="14"/>
-      <c r="C4" s="399"/>
-      <c r="D4" s="399"/>
-      <c r="E4" s="399"/>
-      <c r="F4" s="399"/>
+      <c r="C4" s="388"/>
+      <c r="D4" s="388"/>
+      <c r="E4" s="388"/>
+      <c r="F4" s="388"/>
       <c r="H4" s="16"/>
       <c r="I4" s="17" t="s">
         <v>14</v>
@@ -5985,10 +5979,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="399"/>
-      <c r="D5" s="399"/>
-      <c r="E5" s="399"/>
-      <c r="F5" s="399"/>
+      <c r="C5" s="388"/>
+      <c r="D5" s="388"/>
+      <c r="E5" s="388"/>
+      <c r="F5" s="388"/>
       <c r="K5" s="56"/>
     </row>
     <row r="6" spans="1:12" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6013,10 +6007,10 @@
         <v>0</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="399"/>
-      <c r="D7" s="399"/>
-      <c r="E7" s="399"/>
-      <c r="F7" s="399"/>
+      <c r="C7" s="388"/>
+      <c r="D7" s="388"/>
+      <c r="E7" s="388"/>
+      <c r="F7" s="388"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -6028,10 +6022,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="14"/>
-      <c r="C8" s="399"/>
-      <c r="D8" s="399"/>
-      <c r="E8" s="399"/>
-      <c r="F8" s="399"/>
+      <c r="C8" s="388"/>
+      <c r="D8" s="388"/>
+      <c r="E8" s="388"/>
+      <c r="F8" s="388"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -6043,10 +6037,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="399"/>
-      <c r="D9" s="399"/>
-      <c r="E9" s="399"/>
-      <c r="F9" s="399"/>
+      <c r="C9" s="388"/>
+      <c r="D9" s="388"/>
+      <c r="E9" s="388"/>
+      <c r="F9" s="388"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -6080,215 +6074,215 @@
       <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H12" s="400" t="s">
+      <c r="H12" s="389" t="s">
         <v>42</v>
       </c>
-      <c r="I12" s="401"/>
-      <c r="J12" s="402" t="s">
+      <c r="I12" s="390"/>
+      <c r="J12" s="391" t="s">
         <v>43</v>
       </c>
-      <c r="K12" s="402"/>
-      <c r="L12" s="402"/>
+      <c r="K12" s="391"/>
+      <c r="L12" s="391"/>
     </row>
     <row r="13" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="376" t="s">
+      <c r="A13" s="392" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="382" t="s">
+      <c r="B13" s="395" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="382" t="s">
+      <c r="C13" s="395" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="382"/>
-      <c r="E13" s="382"/>
-      <c r="F13" s="391" t="s">
+      <c r="D13" s="395"/>
+      <c r="E13" s="395"/>
+      <c r="F13" s="397" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="392"/>
+      <c r="G13" s="398"/>
       <c r="H13" s="21"/>
       <c r="I13" s="22"/>
-      <c r="J13" s="393" t="s">
+      <c r="J13" s="379" t="s">
         <v>1</v>
       </c>
-      <c r="K13" s="409"/>
-      <c r="L13" s="405">
+      <c r="K13" s="381"/>
+      <c r="L13" s="375">
         <f>ROUND(K13*0.3,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="377"/>
-      <c r="B14" s="387"/>
-      <c r="C14" s="387" t="s">
+      <c r="A14" s="393"/>
+      <c r="B14" s="396"/>
+      <c r="C14" s="396" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="387"/>
-      <c r="E14" s="387"/>
-      <c r="F14" s="388" t="s">
-        <v>159</v>
-      </c>
-      <c r="G14" s="389"/>
+      <c r="D14" s="396"/>
+      <c r="E14" s="396"/>
+      <c r="F14" s="399" t="s">
+        <v>155</v>
+      </c>
+      <c r="G14" s="400"/>
       <c r="H14" s="24"/>
       <c r="I14" s="25"/>
-      <c r="J14" s="394"/>
-      <c r="K14" s="410"/>
-      <c r="L14" s="406"/>
+      <c r="J14" s="380"/>
+      <c r="K14" s="382"/>
+      <c r="L14" s="376"/>
     </row>
     <row r="15" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="377"/>
-      <c r="B15" s="387"/>
-      <c r="C15" s="387" t="s">
+      <c r="A15" s="393"/>
+      <c r="B15" s="396"/>
+      <c r="C15" s="396" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="387"/>
-      <c r="E15" s="387"/>
-      <c r="F15" s="388" t="s">
+      <c r="D15" s="396"/>
+      <c r="E15" s="396"/>
+      <c r="F15" s="399" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="389"/>
+      <c r="G15" s="400"/>
       <c r="H15" s="27"/>
       <c r="I15" s="28"/>
-      <c r="J15" s="394"/>
-      <c r="K15" s="411"/>
-      <c r="L15" s="406"/>
+      <c r="J15" s="380"/>
+      <c r="K15" s="383"/>
+      <c r="L15" s="376"/>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="377"/>
-      <c r="B16" s="395" t="s">
+      <c r="A16" s="393"/>
+      <c r="B16" s="401" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="387" t="s">
+      <c r="C16" s="396" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="387"/>
-      <c r="E16" s="387"/>
-      <c r="F16" s="388" t="s">
-        <v>160</v>
-      </c>
-      <c r="G16" s="389"/>
+      <c r="D16" s="396"/>
+      <c r="E16" s="396"/>
+      <c r="F16" s="399" t="s">
+        <v>156</v>
+      </c>
+      <c r="G16" s="400"/>
       <c r="H16" s="29"/>
       <c r="I16" s="30"/>
-      <c r="J16" s="394" t="s">
+      <c r="J16" s="380" t="s">
         <v>2</v>
       </c>
-      <c r="K16" s="404"/>
-      <c r="L16" s="406">
+      <c r="K16" s="374"/>
+      <c r="L16" s="376">
         <f>ROUND(K16*0.25,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="377"/>
-      <c r="B17" s="396"/>
-      <c r="C17" s="387" t="s">
+      <c r="A17" s="393"/>
+      <c r="B17" s="402"/>
+      <c r="C17" s="396" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="387"/>
-      <c r="E17" s="387"/>
-      <c r="F17" s="388" t="s">
+      <c r="D17" s="396"/>
+      <c r="E17" s="396"/>
+      <c r="F17" s="399" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="389"/>
+      <c r="G17" s="400"/>
       <c r="H17" s="24"/>
       <c r="I17" s="25"/>
-      <c r="J17" s="394"/>
-      <c r="K17" s="404"/>
-      <c r="L17" s="406"/>
+      <c r="J17" s="380"/>
+      <c r="K17" s="374"/>
+      <c r="L17" s="376"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="378"/>
-      <c r="B18" s="397"/>
-      <c r="C18" s="390" t="s">
+      <c r="A18" s="394"/>
+      <c r="B18" s="403"/>
+      <c r="C18" s="405" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="390"/>
-      <c r="E18" s="390"/>
-      <c r="F18" s="385" t="s">
+      <c r="D18" s="405"/>
+      <c r="E18" s="405"/>
+      <c r="F18" s="386" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="386"/>
+      <c r="G18" s="387"/>
       <c r="H18" s="31"/>
       <c r="I18" s="32"/>
-      <c r="J18" s="398"/>
-      <c r="K18" s="412"/>
-      <c r="L18" s="413"/>
+      <c r="J18" s="404"/>
+      <c r="K18" s="384"/>
+      <c r="L18" s="385"/>
     </row>
     <row r="19" spans="1:12" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="376" t="s">
+      <c r="A19" s="392" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="379" t="s">
+      <c r="B19" s="409" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="382" t="s">
+      <c r="C19" s="395" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="382"/>
-      <c r="E19" s="382"/>
-      <c r="F19" s="383" t="s">
+      <c r="D19" s="395"/>
+      <c r="E19" s="395"/>
+      <c r="F19" s="412" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="384"/>
+      <c r="G19" s="413"/>
       <c r="H19" s="33"/>
       <c r="I19" s="34"/>
-      <c r="J19" s="393" t="s">
-        <v>104</v>
-      </c>
-      <c r="K19" s="403"/>
-      <c r="L19" s="405">
+      <c r="J19" s="379" t="s">
+        <v>100</v>
+      </c>
+      <c r="K19" s="373"/>
+      <c r="L19" s="375">
         <f>ROUND(K19*0.25,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="377"/>
-      <c r="B20" s="380"/>
-      <c r="C20" s="387" t="s">
+      <c r="A20" s="393"/>
+      <c r="B20" s="410"/>
+      <c r="C20" s="396" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="387"/>
-      <c r="E20" s="387"/>
-      <c r="F20" s="388" t="s">
+      <c r="D20" s="396"/>
+      <c r="E20" s="396"/>
+      <c r="F20" s="399" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="389"/>
+      <c r="G20" s="400"/>
       <c r="H20" s="24"/>
       <c r="I20" s="25"/>
-      <c r="J20" s="394"/>
-      <c r="K20" s="404"/>
-      <c r="L20" s="406"/>
+      <c r="J20" s="380"/>
+      <c r="K20" s="374"/>
+      <c r="L20" s="376"/>
     </row>
     <row r="21" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="377"/>
-      <c r="B21" s="381"/>
-      <c r="C21" s="387" t="s">
+      <c r="A21" s="393"/>
+      <c r="B21" s="411"/>
+      <c r="C21" s="396" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="387"/>
-      <c r="E21" s="387"/>
-      <c r="F21" s="388" t="s">
+      <c r="D21" s="396"/>
+      <c r="E21" s="396"/>
+      <c r="F21" s="399" t="s">
         <v>34</v>
       </c>
-      <c r="G21" s="389"/>
+      <c r="G21" s="400"/>
       <c r="H21" s="27"/>
       <c r="I21" s="28"/>
-      <c r="J21" s="394"/>
-      <c r="K21" s="404"/>
-      <c r="L21" s="406"/>
+      <c r="J21" s="380"/>
+      <c r="K21" s="374"/>
+      <c r="L21" s="376"/>
     </row>
     <row r="22" spans="1:12" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="378"/>
+      <c r="A22" s="394"/>
       <c r="B22" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="390"/>
-      <c r="D22" s="390"/>
-      <c r="E22" s="390"/>
-      <c r="F22" s="385" t="s">
+      <c r="C22" s="405"/>
+      <c r="D22" s="405"/>
+      <c r="E22" s="405"/>
+      <c r="F22" s="386" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="386"/>
+      <c r="G22" s="387"/>
       <c r="H22" s="36"/>
       <c r="I22" s="37"/>
       <c r="J22" s="38" t="s">
@@ -6305,21 +6299,21 @@
         <v>37</v>
       </c>
       <c r="B23" s="144" t="s">
-        <v>102</v>
-      </c>
-      <c r="C23" s="373" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="406" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="373"/>
-      <c r="E23" s="373"/>
-      <c r="F23" s="374" t="s">
+      <c r="D23" s="406"/>
+      <c r="E23" s="406"/>
+      <c r="F23" s="407" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="375"/>
+      <c r="G23" s="408"/>
       <c r="H23" s="40"/>
       <c r="I23" s="41"/>
       <c r="J23" s="42" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="K23" s="352"/>
       <c r="L23" s="43">
@@ -6354,11 +6348,11 @@
         <v>6</v>
       </c>
       <c r="J25" s="46"/>
-      <c r="K25" s="407">
+      <c r="K25" s="377">
         <f>SUM(L13:L23)</f>
         <v>0</v>
       </c>
-      <c r="L25" s="408"/>
+      <c r="L25" s="378"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="K26" s="331"/>
@@ -6385,22 +6379,18 @@
     <row r="30" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="K19:K21"/>
-    <mergeCell ref="L19:L21"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="J19:J21"/>
-    <mergeCell ref="K13:K15"/>
-    <mergeCell ref="L13:L15"/>
-    <mergeCell ref="K16:K18"/>
-    <mergeCell ref="L16:L18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="C22:E22"/>
     <mergeCell ref="A13:A18"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="C13:E13"/>
@@ -6417,18 +6407,22 @@
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="K19:K21"/>
+    <mergeCell ref="L19:L21"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="J19:J21"/>
+    <mergeCell ref="K13:K15"/>
+    <mergeCell ref="L13:L15"/>
+    <mergeCell ref="K16:K18"/>
+    <mergeCell ref="L16:L18"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6444,8 +6438,8 @@
   <sheetPr codeName="Blad3"/>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -6472,7 +6466,7 @@
       </c>
       <c r="H2" s="211"/>
       <c r="I2" s="212" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J2" s="213"/>
       <c r="K2" s="214"/>
@@ -6480,11 +6474,11 @@
     </row>
     <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="215" t="s">
-        <v>70</v>
+        <v>190</v>
       </c>
       <c r="H3" s="211"/>
       <c r="I3" s="212" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J3" s="213"/>
       <c r="K3" s="214"/>
@@ -6908,8 +6902,8 @@
   <sheetPr codeName="Blad4"/>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView showZeros="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -6936,7 +6930,7 @@
       </c>
       <c r="H2" s="141"/>
       <c r="I2" s="17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J2" s="18"/>
       <c r="K2" s="142"/>
@@ -6944,11 +6938,11 @@
     </row>
     <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>69</v>
+        <v>190</v>
       </c>
       <c r="H3" s="141"/>
       <c r="I3" s="17" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J3" s="18"/>
       <c r="K3" s="142"/>
@@ -6976,10 +6970,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="399"/>
-      <c r="D5" s="399"/>
-      <c r="E5" s="399"/>
-      <c r="F5" s="399"/>
+      <c r="C5" s="388"/>
+      <c r="D5" s="388"/>
+      <c r="E5" s="388"/>
+      <c r="F5" s="388"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
         <v>14</v>
@@ -6993,10 +6987,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="399"/>
-      <c r="D6" s="399"/>
-      <c r="E6" s="399"/>
-      <c r="F6" s="399"/>
+      <c r="C6" s="388"/>
+      <c r="D6" s="388"/>
+      <c r="E6" s="388"/>
+      <c r="F6" s="388"/>
       <c r="K6" s="56"/>
     </row>
     <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7036,10 +7030,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="399"/>
-      <c r="D9" s="399"/>
-      <c r="E9" s="399"/>
-      <c r="F9" s="399"/>
+      <c r="C9" s="388"/>
+      <c r="D9" s="388"/>
+      <c r="E9" s="388"/>
+      <c r="F9" s="388"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -7051,10 +7045,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="399"/>
-      <c r="D10" s="399"/>
-      <c r="E10" s="399"/>
-      <c r="F10" s="399"/>
+      <c r="C10" s="388"/>
+      <c r="D10" s="388"/>
+      <c r="E10" s="388"/>
+      <c r="F10" s="388"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -7376,8 +7370,8 @@
   <sheetPr codeName="Blad5"/>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -7404,7 +7398,7 @@
       </c>
       <c r="H2" s="141"/>
       <c r="I2" s="17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J2" s="18"/>
       <c r="K2" s="142"/>
@@ -7412,11 +7406,11 @@
     </row>
     <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>68</v>
+        <v>190</v>
       </c>
       <c r="H3" s="141"/>
       <c r="I3" s="17" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J3" s="18"/>
       <c r="K3" s="142"/>
@@ -7444,10 +7438,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="399"/>
-      <c r="D5" s="399"/>
-      <c r="E5" s="399"/>
-      <c r="F5" s="399"/>
+      <c r="C5" s="388"/>
+      <c r="D5" s="388"/>
+      <c r="E5" s="388"/>
+      <c r="F5" s="388"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
         <v>14</v>
@@ -7461,10 +7455,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="399"/>
-      <c r="D6" s="399"/>
-      <c r="E6" s="399"/>
-      <c r="F6" s="399"/>
+      <c r="C6" s="388"/>
+      <c r="D6" s="388"/>
+      <c r="E6" s="388"/>
+      <c r="F6" s="388"/>
       <c r="K6" s="56"/>
     </row>
     <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7504,10 +7498,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="399"/>
-      <c r="D9" s="399"/>
-      <c r="E9" s="399"/>
-      <c r="F9" s="399"/>
+      <c r="C9" s="388"/>
+      <c r="D9" s="388"/>
+      <c r="E9" s="388"/>
+      <c r="F9" s="388"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -7519,10 +7513,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="399"/>
-      <c r="D10" s="399"/>
-      <c r="E10" s="399"/>
-      <c r="F10" s="399"/>
+      <c r="C10" s="388"/>
+      <c r="D10" s="388"/>
+      <c r="E10" s="388"/>
+      <c r="F10" s="388"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -7683,7 +7677,7 @@
     </row>
     <row r="22" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="300" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B22" s="298"/>
       <c r="C22" s="298"/>
@@ -7843,8 +7837,8 @@
   <sheetPr codeName="Blad6"/>
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -7866,11 +7860,11 @@
     <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="210" t="s">
-        <v>71</v>
+        <v>191</v>
       </c>
       <c r="H2" s="211"/>
       <c r="I2" s="212" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J2" s="213"/>
       <c r="K2" s="214"/>
@@ -7878,11 +7872,11 @@
     </row>
     <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="215" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H3" s="211"/>
       <c r="I3" s="212" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J3" s="213"/>
       <c r="K3" s="214"/>
@@ -8004,7 +7998,7 @@
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="223" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B12" s="224"/>
       <c r="C12" s="224"/>
@@ -8064,7 +8058,7 @@
     </row>
     <row r="16" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="236" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B16" s="228"/>
       <c r="C16" s="228"/>
@@ -8089,7 +8083,7 @@
       <c r="I17" s="238"/>
       <c r="J17" s="228"/>
       <c r="K17" s="239" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L17" s="228"/>
     </row>
@@ -8179,12 +8173,12 @@
     </row>
     <row r="24" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="215" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="7" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="113" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C25" s="47"/>
       <c r="D25" s="47"/>
@@ -8198,13 +8192,13 @@
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="243" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C26" s="244"/>
       <c r="D26" s="245"/>
       <c r="E26" s="356"/>
       <c r="F26" s="243" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G26" s="245"/>
       <c r="H26" s="357"/>
@@ -8272,7 +8266,7 @@
     </row>
     <row r="31" spans="1:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G31" s="250" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H31" s="213"/>
       <c r="I31" s="213"/>
@@ -8288,7 +8282,7 @@
     <row r="32" spans="1:12" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="33" spans="1:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I33" s="221" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="J33" s="253"/>
       <c r="K33" s="253"/>
@@ -8340,7 +8334,7 @@
   <sheetPr codeName="Blad7"/>
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
@@ -8994,11 +8988,11 @@
     <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="76" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H2" s="141"/>
       <c r="I2" s="17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J2" s="18"/>
       <c r="K2" s="142"/>
@@ -9006,11 +9000,11 @@
     </row>
     <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H3" s="141"/>
       <c r="I3" s="17" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J3" s="18"/>
       <c r="K3" s="142"/>
@@ -9038,10 +9032,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="399"/>
-      <c r="D5" s="399"/>
-      <c r="E5" s="399"/>
-      <c r="F5" s="399"/>
+      <c r="C5" s="388"/>
+      <c r="D5" s="388"/>
+      <c r="E5" s="388"/>
+      <c r="F5" s="388"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
         <v>14</v>
@@ -9055,10 +9049,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="399"/>
-      <c r="D6" s="399"/>
-      <c r="E6" s="399"/>
-      <c r="F6" s="399"/>
+      <c r="C6" s="388"/>
+      <c r="D6" s="388"/>
+      <c r="E6" s="388"/>
+      <c r="F6" s="388"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -9102,10 +9096,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="399"/>
-      <c r="D9" s="399"/>
-      <c r="E9" s="399"/>
-      <c r="F9" s="399"/>
+      <c r="C9" s="388"/>
+      <c r="D9" s="388"/>
+      <c r="E9" s="388"/>
+      <c r="F9" s="388"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
@@ -9117,10 +9111,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="399"/>
-      <c r="D10" s="399"/>
-      <c r="E10" s="399"/>
-      <c r="F10" s="399"/>
+      <c r="C10" s="388"/>
+      <c r="D10" s="388"/>
+      <c r="E10" s="388"/>
+      <c r="F10" s="388"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
@@ -9136,7 +9130,7 @@
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="90" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B12" s="91"/>
       <c r="C12" s="91"/>
@@ -9196,7 +9190,7 @@
     </row>
     <row r="16" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="98" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B16" s="47"/>
       <c r="C16" s="47"/>
@@ -9218,7 +9212,7 @@
       <c r="F17" s="47"/>
       <c r="G17" s="97"/>
       <c r="H17" s="99" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I17" s="100"/>
       <c r="K17" s="101" t="s">
@@ -9227,7 +9221,7 @@
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="102" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C18" s="80"/>
       <c r="D18" s="81"/>
@@ -9248,7 +9242,7 @@
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="102" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C19" s="80"/>
       <c r="D19" s="81"/>
@@ -9269,7 +9263,7 @@
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="102" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C20" s="80"/>
       <c r="D20" s="81"/>
@@ -9290,13 +9284,13 @@
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="102" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C21" s="80"/>
       <c r="D21" s="81"/>
       <c r="E21" s="359"/>
       <c r="F21" s="147" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G21" s="104"/>
       <c r="H21" s="101"/>
@@ -9308,7 +9302,7 @@
     </row>
     <row r="22" spans="1:12" ht="12.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="106" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C22" s="107"/>
       <c r="D22" s="107"/>
@@ -9319,7 +9313,7 @@
     </row>
     <row r="23" spans="1:12" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G23" s="109" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H23" s="48"/>
       <c r="I23" s="48"/>
@@ -9334,12 +9328,12 @@
     </row>
     <row r="24" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="113" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C25" s="47"/>
       <c r="D25" s="47"/>
@@ -9353,13 +9347,13 @@
     </row>
     <row r="26" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="137" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C26" s="138"/>
       <c r="D26" s="139"/>
       <c r="E26" s="356"/>
       <c r="F26" s="137" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G26" s="139"/>
       <c r="H26" s="123">
@@ -9427,7 +9421,7 @@
     </row>
     <row r="31" spans="1:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G31" s="120" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H31" s="48"/>
       <c r="I31" s="48"/>
@@ -9443,7 +9437,7 @@
     <row r="32" spans="1:12" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="33" spans="1:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I33" s="53" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="J33" s="46"/>
       <c r="K33" s="46"/>
@@ -9491,7 +9485,7 @@
   <sheetPr codeName="Blad8"/>
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B17" sqref="B17:I17"/>
     </sheetView>
   </sheetViews>
@@ -10082,11 +10076,11 @@
     <row r="1" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="76" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H2" s="141"/>
       <c r="I2" s="17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J2" s="18"/>
       <c r="K2" s="142"/>
@@ -10094,11 +10088,11 @@
     </row>
     <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H3" s="141"/>
       <c r="I3" s="17" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J3" s="18"/>
       <c r="K3" s="142"/>
@@ -10126,10 +10120,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="399"/>
-      <c r="D5" s="399"/>
-      <c r="E5" s="399"/>
-      <c r="F5" s="399"/>
+      <c r="C5" s="388"/>
+      <c r="D5" s="388"/>
+      <c r="E5" s="388"/>
+      <c r="F5" s="388"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
         <v>14</v>
@@ -10143,10 +10137,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="399"/>
-      <c r="D6" s="399"/>
-      <c r="E6" s="399"/>
-      <c r="F6" s="399"/>
+      <c r="C6" s="388"/>
+      <c r="D6" s="388"/>
+      <c r="E6" s="388"/>
+      <c r="F6" s="388"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -10190,10 +10184,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="399"/>
-      <c r="D9" s="399"/>
-      <c r="E9" s="399"/>
-      <c r="F9" s="399"/>
+      <c r="C9" s="388"/>
+      <c r="D9" s="388"/>
+      <c r="E9" s="388"/>
+      <c r="F9" s="388"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
@@ -10205,10 +10199,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="399"/>
-      <c r="D10" s="399"/>
-      <c r="E10" s="399"/>
-      <c r="F10" s="399"/>
+      <c r="C10" s="388"/>
+      <c r="D10" s="388"/>
+      <c r="E10" s="388"/>
+      <c r="F10" s="388"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
@@ -10235,16 +10229,16 @@
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="L13" s="12"/>
     </row>
     <row r="14" spans="1:13" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="417" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B14" s="419" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C14" s="420"/>
       <c r="D14" s="420"/>
@@ -10254,7 +10248,7 @@
       <c r="H14" s="420"/>
       <c r="I14" s="421"/>
       <c r="J14" s="23" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="K14" s="361"/>
       <c r="L14" s="335">
@@ -10265,18 +10259,18 @@
     </row>
     <row r="15" spans="1:13" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="418"/>
-      <c r="B15" s="460" t="s">
-        <v>164</v>
-      </c>
-      <c r="C15" s="422"/>
-      <c r="D15" s="422"/>
-      <c r="E15" s="422"/>
-      <c r="F15" s="422"/>
-      <c r="G15" s="422"/>
-      <c r="H15" s="422"/>
-      <c r="I15" s="422"/>
+      <c r="B15" s="422" t="s">
+        <v>160</v>
+      </c>
+      <c r="C15" s="423"/>
+      <c r="D15" s="423"/>
+      <c r="E15" s="423"/>
+      <c r="F15" s="423"/>
+      <c r="G15" s="423"/>
+      <c r="H15" s="423"/>
+      <c r="I15" s="423"/>
       <c r="J15" s="38" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="K15" s="362"/>
       <c r="L15" s="339">
@@ -10286,20 +10280,20 @@
     </row>
     <row r="16" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="417" t="s">
-        <v>178</v>
-      </c>
-      <c r="B16" s="424" t="s">
-        <v>165</v>
-      </c>
-      <c r="C16" s="425"/>
-      <c r="D16" s="425"/>
-      <c r="E16" s="425"/>
-      <c r="F16" s="425"/>
-      <c r="G16" s="425"/>
-      <c r="H16" s="425"/>
-      <c r="I16" s="425"/>
+        <v>174</v>
+      </c>
+      <c r="B16" s="425" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16" s="426"/>
+      <c r="D16" s="426"/>
+      <c r="E16" s="426"/>
+      <c r="F16" s="426"/>
+      <c r="G16" s="426"/>
+      <c r="H16" s="426"/>
+      <c r="I16" s="426"/>
       <c r="J16" s="23" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K16" s="363"/>
       <c r="L16" s="336">
@@ -10308,17 +10302,17 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="423"/>
-      <c r="B17" s="426" t="s">
-        <v>193</v>
-      </c>
-      <c r="C17" s="427"/>
-      <c r="D17" s="427"/>
-      <c r="E17" s="427"/>
-      <c r="F17" s="427"/>
-      <c r="G17" s="427"/>
-      <c r="H17" s="427"/>
-      <c r="I17" s="427"/>
+      <c r="A17" s="424"/>
+      <c r="B17" s="427" t="s">
+        <v>189</v>
+      </c>
+      <c r="C17" s="428"/>
+      <c r="D17" s="428"/>
+      <c r="E17" s="428"/>
+      <c r="F17" s="428"/>
+      <c r="G17" s="428"/>
+      <c r="H17" s="428"/>
+      <c r="I17" s="428"/>
       <c r="J17" s="26" t="s">
         <v>4</v>
       </c>
@@ -10330,18 +10324,18 @@
     </row>
     <row r="18" spans="1:13" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="418"/>
-      <c r="B18" s="428" t="s">
-        <v>92</v>
-      </c>
-      <c r="C18" s="422"/>
-      <c r="D18" s="422"/>
-      <c r="E18" s="422"/>
-      <c r="F18" s="422"/>
-      <c r="G18" s="422"/>
-      <c r="H18" s="422"/>
-      <c r="I18" s="422"/>
+      <c r="B18" s="429" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="423"/>
+      <c r="D18" s="423"/>
+      <c r="E18" s="423"/>
+      <c r="F18" s="423"/>
+      <c r="G18" s="423"/>
+      <c r="H18" s="423"/>
+      <c r="I18" s="423"/>
       <c r="J18" s="38" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="K18" s="365"/>
       <c r="L18" s="338">
@@ -10385,7 +10379,7 @@
     <row r="21" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="44"/>
       <c r="B21" s="80" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C21" s="81"/>
       <c r="D21" s="82"/>
@@ -10402,7 +10396,7 @@
     <row r="22" spans="1:13" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="23" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I23" s="45" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J23" s="46"/>
       <c r="K23" s="46"/>
@@ -10458,6 +10452,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C10:F10"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:I14"/>
     <mergeCell ref="B15:I15"/>
@@ -10465,11 +10464,6 @@
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="B18:I18"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10487,7 +10481,7 @@
   </sheetPr>
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -10508,11 +10502,11 @@
     <row r="1" spans="1:13" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="55" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H2" s="141"/>
       <c r="I2" s="17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J2" s="18"/>
       <c r="K2" s="142"/>
@@ -10520,11 +10514,11 @@
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H3" s="141"/>
       <c r="I3" s="17" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J3" s="18"/>
       <c r="K3" s="142"/>
@@ -10552,10 +10546,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="399"/>
-      <c r="D5" s="399"/>
-      <c r="E5" s="399"/>
-      <c r="F5" s="399"/>
+      <c r="C5" s="388"/>
+      <c r="D5" s="388"/>
+      <c r="E5" s="388"/>
+      <c r="F5" s="388"/>
       <c r="H5" s="141"/>
       <c r="I5" s="17" t="s">
         <v>14</v>
@@ -10569,10 +10563,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="399"/>
-      <c r="D6" s="399"/>
-      <c r="E6" s="399"/>
-      <c r="F6" s="399"/>
+      <c r="C6" s="388"/>
+      <c r="D6" s="388"/>
+      <c r="E6" s="388"/>
+      <c r="F6" s="388"/>
       <c r="K6" s="56"/>
     </row>
     <row r="7" spans="1:13" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -10612,10 +10606,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="14"/>
-      <c r="C9" s="399"/>
-      <c r="D9" s="399"/>
-      <c r="E9" s="399"/>
-      <c r="F9" s="399"/>
+      <c r="C9" s="388"/>
+      <c r="D9" s="388"/>
+      <c r="E9" s="388"/>
+      <c r="F9" s="388"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -10627,10 +10621,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="C10" s="399"/>
-      <c r="D10" s="399"/>
-      <c r="E10" s="399"/>
-      <c r="F10" s="399"/>
+      <c r="C10" s="388"/>
+      <c r="D10" s="388"/>
+      <c r="E10" s="388"/>
+      <c r="F10" s="388"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -10660,7 +10654,7 @@
     </row>
     <row r="14" spans="1:13" s="2" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="148" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B14" s="149"/>
       <c r="C14" s="149"/>
@@ -10680,14 +10674,14 @@
       <c r="M14" s="52"/>
     </row>
     <row r="15" spans="1:13" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="429" t="s">
-        <v>109</v>
-      </c>
-      <c r="B15" s="430"/>
-      <c r="C15" s="430"/>
-      <c r="D15" s="430"/>
-      <c r="E15" s="430"/>
-      <c r="F15" s="431"/>
+      <c r="A15" s="430" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="431"/>
+      <c r="C15" s="431"/>
+      <c r="D15" s="431"/>
+      <c r="E15" s="431"/>
+      <c r="F15" s="432"/>
       <c r="G15" s="59"/>
       <c r="H15" s="59"/>
       <c r="I15" s="14"/>
@@ -10696,14 +10690,14 @@
       <c r="L15" s="354"/>
     </row>
     <row r="16" spans="1:13" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="429" t="s">
-        <v>110</v>
-      </c>
-      <c r="B16" s="430"/>
-      <c r="C16" s="430"/>
-      <c r="D16" s="430"/>
-      <c r="E16" s="430"/>
-      <c r="F16" s="431"/>
+      <c r="A16" s="430" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="431"/>
+      <c r="C16" s="431"/>
+      <c r="D16" s="431"/>
+      <c r="E16" s="431"/>
+      <c r="F16" s="432"/>
       <c r="G16" s="59"/>
       <c r="H16" s="59"/>
       <c r="I16" s="14"/>
@@ -10713,7 +10707,7 @@
     </row>
     <row r="17" spans="1:18" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="300" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B17" s="301"/>
       <c r="C17" s="301"/>
@@ -10729,7 +10723,7 @@
     </row>
     <row r="18" spans="1:18" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="300" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B18" s="301"/>
       <c r="C18" s="301"/>
@@ -10745,7 +10739,7 @@
     </row>
     <row r="19" spans="1:18" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="300" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B19" s="301"/>
       <c r="C19" s="301"/>
@@ -10764,27 +10758,27 @@
       <c r="L20" s="182"/>
     </row>
     <row r="21" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="435" t="s">
-        <v>114</v>
-      </c>
-      <c r="B21" s="436"/>
-      <c r="C21" s="436"/>
-      <c r="D21" s="436"/>
-      <c r="E21" s="436"/>
-      <c r="F21" s="436"/>
-      <c r="G21" s="436"/>
-      <c r="H21" s="436"/>
-      <c r="I21" s="436"/>
+      <c r="A21" s="436" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" s="437"/>
+      <c r="C21" s="437"/>
+      <c r="D21" s="437"/>
+      <c r="E21" s="437"/>
+      <c r="F21" s="437"/>
+      <c r="G21" s="437"/>
+      <c r="H21" s="437"/>
+      <c r="I21" s="437"/>
       <c r="J21" s="181"/>
       <c r="K21" s="180"/>
       <c r="L21" s="10"/>
       <c r="R21" s="175"/>
     </row>
     <row r="22" spans="1:18" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="443" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" s="444"/>
+      <c r="A22" s="444" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="445"/>
       <c r="C22" s="179"/>
       <c r="D22" s="179"/>
       <c r="E22" s="179"/>
@@ -10799,28 +10793,28 @@
       <c r="R22" s="175"/>
     </row>
     <row r="23" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="439" t="s">
-        <v>97</v>
-      </c>
-      <c r="B23" s="440"/>
+      <c r="A23" s="440" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="441"/>
       <c r="C23" s="366"/>
-      <c r="D23" s="437" t="s">
-        <v>85</v>
-      </c>
-      <c r="E23" s="438"/>
+      <c r="D23" s="438" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="439"/>
       <c r="F23" s="367"/>
       <c r="G23" s="308" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H23" s="309">
         <f>IFERROR(IF(ROUND(C23/F23,3)&gt;10,10,ROUND(C23/F23,3)),10)</f>
         <v>10</v>
       </c>
       <c r="I23" s="310" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="J23" s="308" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K23" s="311">
         <f>10-H23</f>
@@ -10830,11 +10824,11 @@
       <c r="R23" s="175"/>
     </row>
     <row r="24" spans="1:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="441" t="s">
+      <c r="A24" s="442" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="442"/>
-      <c r="C24" s="442"/>
+      <c r="B24" s="443"/>
+      <c r="C24" s="443"/>
       <c r="D24" s="312"/>
       <c r="E24" s="312"/>
       <c r="F24" s="312"/>
@@ -10846,19 +10840,19 @@
       <c r="R24" s="175"/>
     </row>
     <row r="25" spans="1:18" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="432" t="s">
-        <v>99</v>
-      </c>
-      <c r="B25" s="433"/>
-      <c r="C25" s="433"/>
-      <c r="D25" s="433"/>
-      <c r="E25" s="433"/>
-      <c r="F25" s="433"/>
-      <c r="G25" s="433"/>
-      <c r="H25" s="433"/>
-      <c r="I25" s="433"/>
-      <c r="J25" s="433"/>
-      <c r="K25" s="434"/>
+      <c r="A25" s="433" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="434"/>
+      <c r="C25" s="434"/>
+      <c r="D25" s="434"/>
+      <c r="E25" s="434"/>
+      <c r="F25" s="434"/>
+      <c r="G25" s="434"/>
+      <c r="H25" s="434"/>
+      <c r="I25" s="434"/>
+      <c r="J25" s="434"/>
+      <c r="K25" s="435"/>
       <c r="L25" s="11">
         <f>IFERROR(K23-K24,0)</f>
         <v>0</v>
@@ -10905,7 +10899,7 @@
     </row>
     <row r="28" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L28" s="168" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -10920,7 +10914,7 @@
     <row r="30" spans="1:18" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H30" s="165"/>
       <c r="I30" s="164" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J30" s="163"/>
       <c r="K30" s="162"/>
@@ -11020,24 +11014,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100570C130F412EDB4EBF3E80DF6A9149FD" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfaa3b10b9be17ef9f56bd19dc71004c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddb0c952b897a810c8a4e377cff6bff8" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -11103,10 +11079,37 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A00BD0D-8423-4FFE-92A4-D273D2078383}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11127,18 +11130,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A00BD0D-8423-4FFE-92A4-D273D2078383}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>